<commit_message>
Kompatibilität mit Win7 und anderen Installations-Orten erhöht - Vorlagencache wird jetzt als eine einzige Datei in TEMP-Ordner geschrieben. - Konfiguration und Hilfe werden jetzt nicht mehr im übergeordneten verzeichnis gesucht, sondern im Unterverzeichnis "GeoToolsRes".
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -11,7 +11,7 @@
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$114</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -42,7 +42,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Sinnvoll sind nur Variablennamen, die auch im Programmkode vereinbart sind.</t>
         </r>
@@ -65,7 +65,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Gültige Ja/Nein-Werte:
@@ -127,6 +127,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 [ANSCHRIFT]
@@ -169,7 +170,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> ohne Bedeutung </t>
         </r>
@@ -201,7 +202,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 1. Er darf nicht beginnen mit: "S.", "F.", "V."
@@ -217,7 +218,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Beschreibung ist frei wählbar
 </t>
@@ -252,7 +253,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Laenge
@@ -283,7 +284,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Kategorie des Spaltennamens 
 - siehe oben Punkt 2.</t>
@@ -298,7 +299,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Kategorie Name ist frei wählbar
 </t>
@@ -313,7 +314,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">... siehe Beschreibung oben, Punkt 2.
 </t>
@@ -325,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="394">
   <si>
     <t>GK.X</t>
   </si>
@@ -411,9 +412,6 @@
     <t>SO-Höhe</t>
   </si>
   <si>
-    <t>Überhöhung</t>
-  </si>
-  <si>
     <t>Hebung der unteren Schiene in der Schere</t>
   </si>
   <si>
@@ -663,15 +661,6 @@
     <t>Kleinkoo' mittlerer Fehler Höhe</t>
   </si>
   <si>
-    <t>Bezug.StrNr</t>
-  </si>
-  <si>
-    <t>Bezug.StrBez</t>
-  </si>
-  <si>
-    <t>Bezug.RiKz</t>
-  </si>
-  <si>
     <t>Bezug.Auftrag</t>
   </si>
   <si>
@@ -712,9 +701,6 @@
   </si>
   <si>
     <t>Vermarkung Art (Text)</t>
-  </si>
-  <si>
-    <t>Richtungskennzeichen Gleis</t>
   </si>
   <si>
     <t>Bezug.Hoe.SysText</t>
@@ -868,6 +854,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> vor oder nur als Zahl?</t>
     </r>
@@ -1311,12 +1298,318 @@
   <si>
     <t>Status des Kilometers (TK.Km)</t>
   </si>
+  <si>
+    <t>Pkt.Att1.Kode</t>
+  </si>
+  <si>
+    <t>Attribut-1 Kode</t>
+  </si>
+  <si>
+    <t>Pkt.Att1.Text</t>
+  </si>
+  <si>
+    <t>Attribut-1 Text</t>
+  </si>
+  <si>
+    <t>Pkt.Att2.Kode</t>
+  </si>
+  <si>
+    <t>Attribut-2 Kode</t>
+  </si>
+  <si>
+    <t>Pkt.Att2.Text</t>
+  </si>
+  <si>
+    <t>Attribut-2 Text</t>
+  </si>
+  <si>
+    <t>Pkt.Att3.Kode</t>
+  </si>
+  <si>
+    <t>Attribut-3 Kode</t>
+  </si>
+  <si>
+    <t>Pkt.Att3.Text</t>
+  </si>
+  <si>
+    <t>Attribut-3 Text</t>
+  </si>
+  <si>
+    <t>Pkt.Att4.Kode</t>
+  </si>
+  <si>
+    <t>Attribut-4 Kode</t>
+  </si>
+  <si>
+    <t>Pkt.Att4.Text</t>
+  </si>
+  <si>
+    <t>Attribut-4 Text</t>
+  </si>
+  <si>
+    <t>Pkt.Att5.Kode</t>
+  </si>
+  <si>
+    <t>Attribut-5 Kode</t>
+  </si>
+  <si>
+    <t>Pkt.Att5.Text</t>
+  </si>
+  <si>
+    <t>Attribut-5 Text</t>
+  </si>
+  <si>
+    <t>Bezug.Zeit</t>
+  </si>
+  <si>
+    <t>Zeitstempel</t>
+  </si>
+  <si>
+    <t>Kode.AD.Exz</t>
+  </si>
+  <si>
+    <t>AD-Kode Exzentrum</t>
+  </si>
+  <si>
+    <t>Bezug.Bahn.RiKz</t>
+  </si>
+  <si>
+    <t>Bezug.Bahn.StrBez</t>
+  </si>
+  <si>
+    <t>Bezug.Bahn.StrNr</t>
+  </si>
+  <si>
+    <t>Gleis Richtungskennzeichen</t>
+  </si>
+  <si>
+    <t>Gleis Bezeichnung (Nummer)</t>
+  </si>
+  <si>
+    <t>Bezug.Bahn.StrZone</t>
+  </si>
+  <si>
+    <t>Strecke Bereich/Abschnitt</t>
+  </si>
+  <si>
+    <t>Bezug.Bahn.Gleis</t>
+  </si>
+  <si>
+    <t>TK.KmText</t>
+  </si>
+  <si>
+    <t>Kilometer als Kilometerschreibweise</t>
+  </si>
+  <si>
+    <t>Herkunft</t>
+  </si>
+  <si>
+    <t>Orig.Mess.Datum</t>
+  </si>
+  <si>
+    <t>Orig.Mess.Name</t>
+  </si>
+  <si>
+    <t>Orig.Erst.Datum</t>
+  </si>
+  <si>
+    <t>Orig.Erst.Name</t>
+  </si>
+  <si>
+    <t>Orig.Aend.Datum</t>
+  </si>
+  <si>
+    <t>Orig.Aend.Name</t>
+  </si>
+  <si>
+    <t>Orig.Pruef.Datum</t>
+  </si>
+  <si>
+    <t>Orig.Pruef.Name</t>
+  </si>
+  <si>
+    <t>Herkunft Messung Datum</t>
+  </si>
+  <si>
+    <t>Herkunft Messung Name</t>
+  </si>
+  <si>
+    <t>Herkunft Erstellung Datum</t>
+  </si>
+  <si>
+    <t>Herkunft Erstellung Name</t>
+  </si>
+  <si>
+    <t>Herkunft Aenderung Datum</t>
+  </si>
+  <si>
+    <t>Herkunft Aenderung Name</t>
+  </si>
+  <si>
+    <t>Herkunft Pruefung Datum</t>
+  </si>
+  <si>
+    <t>Herkunft Pruefung Name</t>
+  </si>
+  <si>
+    <t>Überhöhung ("+" = normal, "-" = invers)</t>
+  </si>
+  <si>
+    <t>Überhöhung absolut ("+" = li. Schiene üb.)</t>
+  </si>
+  <si>
+    <t>Tra.ua</t>
+  </si>
+  <si>
+    <t>TK.Seite</t>
+  </si>
+  <si>
+    <t>Seitl. Lage zur Achse, z.B.: L, R, +, -, re</t>
+  </si>
+  <si>
+    <t>Lichtraumprüfung</t>
+  </si>
+  <si>
+    <t>Messung</t>
+  </si>
+  <si>
+    <t>Messung Bildname</t>
+  </si>
+  <si>
+    <t>Messung Bildnummer</t>
+  </si>
+  <si>
+    <t>Messung Art</t>
+  </si>
+  <si>
+    <t>Mess.BildName</t>
+  </si>
+  <si>
+    <t>Mess.BildNr</t>
+  </si>
+  <si>
+    <t>Mess.Art</t>
+  </si>
+  <si>
+    <t>Messung PELIM CD-BildNr</t>
+  </si>
+  <si>
+    <t>Messung PELIM CD-Nr</t>
+  </si>
+  <si>
+    <t>Messung PELIM RahmenNr</t>
+  </si>
+  <si>
+    <t>Messung PELIM Version</t>
+  </si>
+  <si>
+    <t>Mess.PELIM.CDBildNr</t>
+  </si>
+  <si>
+    <t>Mess.PELIM.CDNr</t>
+  </si>
+  <si>
+    <t>Mess.PELIM.RahmenNr</t>
+  </si>
+  <si>
+    <t>Mess.PELIM.Version</t>
+  </si>
+  <si>
+    <t>LRP.Konfig.Regelwerk</t>
+  </si>
+  <si>
+    <t>LRP.Konfig.Profil</t>
+  </si>
+  <si>
+    <t>LRP.Konfig.GrzBasis</t>
+  </si>
+  <si>
+    <t>LRP.Konfig.LinRes</t>
+  </si>
+  <si>
+    <t>LRP Konfig Regelwerk</t>
+  </si>
+  <si>
+    <t>LRP Konfig Lichtraum</t>
+  </si>
+  <si>
+    <t>LRP Konfig GrenzlinienBasis</t>
+  </si>
+  <si>
+    <t>LRP Konfig Linienauflösung</t>
+  </si>
+  <si>
+    <t>LRP Einragung Abstand</t>
+  </si>
+  <si>
+    <t>LRP Einragung Höhe</t>
+  </si>
+  <si>
+    <t>LRP Einragung Betrag</t>
+  </si>
+  <si>
+    <t>LRP Einragung Bereich</t>
+  </si>
+  <si>
+    <t>LRP Einragung Lichtraum</t>
+  </si>
+  <si>
+    <t>LRP.Einragg.QG</t>
+  </si>
+  <si>
+    <t>LRP.Einragg.HG</t>
+  </si>
+  <si>
+    <t>LRP.Einragg.Betrag</t>
+  </si>
+  <si>
+    <t>LRP.Einragg.Lichtraum</t>
+  </si>
+  <si>
+    <t>LRP.Einragg.Bereich</t>
+  </si>
+  <si>
+    <t>Tra.maxV</t>
+  </si>
+  <si>
+    <t>Tra.uf</t>
+  </si>
+  <si>
+    <t>Überhöhungsfehlbetrag</t>
+  </si>
+  <si>
+    <t>Maximalgeschwindigkeit</t>
+  </si>
+  <si>
+    <t>LRP.ID</t>
+  </si>
+  <si>
+    <t>LRP.Typ</t>
+  </si>
+  <si>
+    <t>LRP ID</t>
+  </si>
+  <si>
+    <t>LRP Typ</t>
+  </si>
+  <si>
+    <t>Mess.Methode</t>
+  </si>
+  <si>
+    <t>Messung Methode</t>
+  </si>
+  <si>
+    <t>Messung AufnahmeNr</t>
+  </si>
+  <si>
+    <t>Mess.AufnahmeID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1355,16 +1648,9 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1378,12 +1664,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color indexed="62"/>
@@ -1393,12 +1673,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1782,7 +2057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1809,13 +2084,13 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1924,10 +2199,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8678333" y="0"/>
+          <a:off x="8805333" y="0"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="731" y="0"/>
-          <a:chExt cx="8677602" cy="450"/>
+          <a:chExt cx="8804602" cy="450"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -1980,7 +2255,7 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="8678333" y="0"/>
+                <a:off x="8805333" y="0"/>
                 <a:ext cx="0" cy="0"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -3109,148 +3384,148 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>157</v>
-      </c>
       <c r="C9" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3258,7 +3533,7 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -3273,16 +3548,16 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="37" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.90625" style="3" customWidth="1"/>
@@ -3293,7 +3568,7 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -3305,7 +3580,7 @@
     <row r="2" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="18" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
@@ -3316,7 +3591,7 @@
     <row r="3" spans="1:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="39"/>
@@ -3327,7 +3602,7 @@
     <row r="4" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="18" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -3338,7 +3613,7 @@
     <row r="5" spans="1:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="37" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="39"/>
@@ -3349,7 +3624,7 @@
     <row r="6" spans="1:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="39"/>
@@ -3360,7 +3635,7 @@
     <row r="7" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
       <c r="B7" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
@@ -3371,7 +3646,7 @@
     <row r="8" spans="1:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="39"/>
@@ -3382,7 +3657,7 @@
     <row r="9" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
@@ -3393,7 +3668,7 @@
     <row r="10" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
@@ -3404,7 +3679,7 @@
     <row r="11" spans="1:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="37" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
@@ -3423,19 +3698,19 @@
     </row>
     <row r="13" spans="1:7" s="11" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F13" s="50" t="s">
         <v>22</v>
@@ -3444,17 +3719,17 @@
     </row>
     <row r="14" spans="1:7" s="12" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
       <c r="F14" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
@@ -3462,402 +3737,402 @@
         <v>1</v>
       </c>
       <c r="B15" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>69</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
       <c r="F15" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26">
         <v>3</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26">
         <v>5</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>7</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26">
         <v>8</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
       <c r="F22" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>9</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
       <c r="F23" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
         <v>10</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G24" s="30"/>
     </row>
-    <row r="25" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
         <v>11</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="30"/>
     </row>
-    <row r="26" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>12</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" s="30"/>
     </row>
-    <row r="27" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26">
         <v>13</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
       <c r="F27" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>14</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26">
         <v>15</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" s="30"/>
     </row>
-    <row r="30" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>16</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>17</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26">
         <v>18</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" s="30"/>
     </row>
-    <row r="33" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26">
         <v>19</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" s="30"/>
     </row>
-    <row r="34" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26">
+    <row r="34" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>20</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G34" s="30"/>
     </row>
-    <row r="35" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26">
         <v>21</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" s="30"/>
     </row>
-    <row r="36" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>22</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G36" s="30"/>
     </row>
-    <row r="37" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
         <v>23</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G37" s="30"/>
     </row>
-    <row r="38" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>24</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>26</v>
@@ -3865,1829 +4140,2719 @@
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
       <c r="F38" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G38" s="30"/>
     </row>
-    <row r="39" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26">
         <v>25</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D39" s="28"/>
       <c r="E39" s="28"/>
       <c r="F39" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G39" s="30"/>
     </row>
-    <row r="40" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>26</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D40" s="28"/>
       <c r="E40" s="28"/>
       <c r="F40" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G40" s="30"/>
     </row>
-    <row r="41" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>27</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>115</v>
+        <v>292</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>87</v>
+        <v>293</v>
       </c>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26">
         <v>28</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>118</v>
+        <v>294</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>116</v>
+        <v>295</v>
       </c>
       <c r="D42" s="28"/>
       <c r="E42" s="28"/>
       <c r="F42" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G42" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+        <v>65</v>
+      </c>
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26">
         <v>29</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>119</v>
+        <v>296</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>117</v>
+        <v>297</v>
       </c>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G43" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26">
+        <v>65</v>
+      </c>
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>30</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>135</v>
+        <v>298</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>86</v>
+        <v>299</v>
       </c>
       <c r="D44" s="28"/>
       <c r="E44" s="28"/>
       <c r="F44" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+        <v>65</v>
+      </c>
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="26">
         <v>31</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>136</v>
+        <v>301</v>
       </c>
       <c r="D45" s="28"/>
       <c r="E45" s="28"/>
       <c r="F45" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G45" s="30"/>
+    </row>
+    <row r="46" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>32</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>131</v>
+        <v>302</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>137</v>
+        <v>303</v>
       </c>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26">
         <v>33</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>132</v>
+        <v>304</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>139</v>
+        <v>305</v>
       </c>
       <c r="D47" s="28"/>
       <c r="E47" s="28"/>
       <c r="F47" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G47" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>34</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>133</v>
+        <v>306</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>138</v>
+        <v>307</v>
       </c>
       <c r="D48" s="28"/>
       <c r="E48" s="28"/>
       <c r="F48" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26">
         <v>35</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>134</v>
+        <v>308</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>85</v>
+        <v>309</v>
       </c>
       <c r="D49" s="28"/>
       <c r="E49" s="28"/>
       <c r="F49" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G49" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="50" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>36</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>114</v>
+        <v>310</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>129</v>
+        <v>311</v>
       </c>
       <c r="D50" s="28"/>
       <c r="E50" s="28"/>
       <c r="F50" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G50" s="30"/>
+    </row>
+    <row r="51" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>37</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D51" s="28"/>
       <c r="E51" s="28"/>
       <c r="F51" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="26">
         <v>38</v>
       </c>
       <c r="B52" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="28" t="s">
         <v>112</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>88</v>
       </c>
       <c r="D52" s="28"/>
       <c r="E52" s="28"/>
       <c r="F52" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G52" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="26">
         <v>39</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D53" s="28"/>
       <c r="E53" s="28"/>
       <c r="F53" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G53" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>40</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D54" s="28"/>
       <c r="E54" s="28"/>
       <c r="F54" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G54" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="26">
         <v>41</v>
       </c>
       <c r="B55" s="27" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D55" s="28"/>
       <c r="E55" s="28"/>
       <c r="F55" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G55" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>224</v>
+        <v>126</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D56" s="28"/>
       <c r="E56" s="28"/>
       <c r="F56" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G56" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="26">
         <v>43</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="D57" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="D57" s="28"/>
       <c r="E57" s="28"/>
       <c r="F57" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G57" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D58" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D58" s="28"/>
       <c r="E58" s="28"/>
       <c r="F58" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G58" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="26">
         <v>45</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D59" s="28"/>
       <c r="E59" s="28"/>
       <c r="F59" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G59" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>46</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>98</v>
+        <v>312</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="D60" s="28"/>
       <c r="E60" s="28"/>
       <c r="F60" s="29" t="s">
-        <v>23</v>
+        <v>184</v>
       </c>
       <c r="G60" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>47</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>6</v>
+        <v>323</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61" s="28" t="s">
-        <v>11</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
       <c r="F61" s="29" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="G61" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="26">
         <v>48</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="D62" s="28"/>
       <c r="E62" s="28"/>
       <c r="F62" s="29" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="G62" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="26">
         <v>49</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>11</v>
+        <v>317</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E63" s="28" t="s">
-        <v>6</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="29" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="G63" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>50</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>8</v>
+        <v>318</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D64" s="28"/>
       <c r="E64" s="28"/>
       <c r="F64" s="29" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="G64" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>51</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="D65" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="D65" s="28"/>
       <c r="E65" s="28"/>
       <c r="F65" s="29" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="G65" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26">
         <v>52</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" s="28"/>
       <c r="F66" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G66" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>53</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" s="28"/>
       <c r="F67" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G67" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="26">
         <v>54</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>285</v>
+        <v>91</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E68" s="28"/>
       <c r="F68" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G68" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>55</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>284</v>
+        <v>219</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>286</v>
+        <v>220</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E69" s="28"/>
       <c r="F69" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G69" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="26">
         <v>56</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>287</v>
+        <v>96</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>292</v>
+        <v>102</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70" s="28"/>
       <c r="F70" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G70" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>57</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>288</v>
+        <v>95</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>293</v>
+        <v>101</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E71" s="28"/>
       <c r="F71" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G71" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>58</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>289</v>
+        <v>98</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>294</v>
+        <v>100</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E72" s="28"/>
       <c r="F72" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G72" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="26">
         <v>59</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>290</v>
+        <v>97</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>295</v>
+        <v>99</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E73" s="28"/>
       <c r="F73" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="26">
         <v>60</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E74" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="E74" s="28" t="s">
+        <v>11</v>
+      </c>
       <c r="F74" s="29" t="s">
         <v>24</v>
       </c>
       <c r="G74" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>61</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D75" s="28"/>
       <c r="E75" s="28"/>
       <c r="F75" s="29" t="s">
         <v>24</v>
       </c>
       <c r="G75" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>62</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>7</v>
+        <v>324</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="D76" s="28"/>
       <c r="E76" s="28"/>
       <c r="F76" s="29" t="s">
         <v>24</v>
       </c>
       <c r="G76" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="26">
         <v>63</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E77" s="28"/>
+        <v>48</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="F77" s="29" t="s">
         <v>24</v>
       </c>
       <c r="G77" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>64</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>12</v>
+        <v>346</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D78" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="D78" s="28"/>
       <c r="E78" s="28"/>
       <c r="F78" s="29" t="s">
         <v>24</v>
       </c>
       <c r="G78" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="26">
         <v>65</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E79" s="28"/>
       <c r="F79" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G79" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>66</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E80" s="28"/>
       <c r="F80" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G80" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="26">
         <v>67</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E81" s="28"/>
       <c r="F81" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G81" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>68</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E82" s="28"/>
       <c r="F82" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G82" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>69</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>108</v>
+        <v>278</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>109</v>
+        <v>280</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E83" s="28"/>
       <c r="F83" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G83" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="26">
         <v>70</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>106</v>
+        <v>279</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>107</v>
+        <v>281</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E84" s="28"/>
       <c r="F84" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G84" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="26">
         <v>71</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>104</v>
+        <v>282</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>105</v>
+        <v>287</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E85" s="28"/>
       <c r="F85" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G85" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>72</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>14</v>
+        <v>283</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D86" s="28"/>
+        <v>288</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E86" s="28"/>
       <c r="F86" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G86" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>73</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>15</v>
+        <v>284</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87" s="28"/>
+        <v>289</v>
+      </c>
+      <c r="D87" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E87" s="28"/>
       <c r="F87" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G87" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="26">
         <v>74</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>13</v>
+        <v>285</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D88" s="28"/>
+        <v>290</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E88" s="28"/>
       <c r="F88" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G88" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>75</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D89" s="28"/>
+        <v>36</v>
+      </c>
+      <c r="D89" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E89" s="28"/>
       <c r="F89" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G89" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="26">
         <v>76</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="D90" s="28"/>
+        <v>37</v>
+      </c>
+      <c r="D90" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E90" s="28"/>
       <c r="F90" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G90" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>77</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>171</v>
+        <v>7</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="D91" s="28"/>
+        <v>40</v>
+      </c>
+      <c r="D91" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E91" s="28"/>
       <c r="F91" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G91" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="26">
         <v>78</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>277</v>
+        <v>10</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>279</v>
-      </c>
-      <c r="D92" s="28"/>
+        <v>39</v>
+      </c>
+      <c r="D92" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E92" s="28"/>
       <c r="F92" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G92" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>79</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>278</v>
+        <v>12</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="D93" s="28"/>
+        <v>38</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E93" s="28"/>
       <c r="F93" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G93" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>80</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E94" s="28"/>
       <c r="F94" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G94" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="26">
         <v>81</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E95" s="28"/>
       <c r="F95" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G95" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="26">
         <v>82</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E96" s="28"/>
       <c r="F96" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G96" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>83</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E97" s="28"/>
       <c r="F97" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G97" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>84</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E98" s="28"/>
       <c r="F98" s="29" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="G98" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="26">
         <v>85</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>268</v>
+        <v>105</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E99" s="28"/>
       <c r="F99" s="29" t="s">
-        <v>272</v>
+        <v>72</v>
       </c>
       <c r="G99" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>86</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>269</v>
+        <v>103</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>271</v>
+        <v>104</v>
       </c>
       <c r="D100" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E100" s="28"/>
       <c r="F100" s="29" t="s">
-        <v>272</v>
+        <v>72</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="26">
         <v>87</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>273</v>
+        <v>14</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>274</v>
+        <v>44</v>
       </c>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
       <c r="F101" s="29" t="s">
-        <v>272</v>
+        <v>25</v>
       </c>
       <c r="G101" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>88</v>
       </c>
       <c r="B102" s="27" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>221</v>
+        <v>45</v>
       </c>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
       <c r="F102" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="26">
         <v>89</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
       <c r="F103" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>90</v>
       </c>
       <c r="B104" s="27" t="s">
-        <v>249</v>
+        <v>16</v>
       </c>
       <c r="C104" s="28" t="s">
-        <v>234</v>
+        <v>46</v>
       </c>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
       <c r="F104" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G104" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>91</v>
       </c>
       <c r="B105" s="27" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
       <c r="F105" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G105" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="26">
         <v>92</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>228</v>
+        <v>166</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>229</v>
+        <v>276</v>
       </c>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
       <c r="F106" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G106" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="26">
         <v>93</v>
       </c>
       <c r="B107" s="27" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="C107" s="28" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
       <c r="F107" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G107" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>94</v>
       </c>
       <c r="B108" s="27" t="s">
-        <v>226</v>
+        <v>273</v>
       </c>
       <c r="C108" s="28" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
       <c r="F108" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>95</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>232</v>
+        <v>17</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>233</v>
+        <v>29</v>
       </c>
       <c r="D109" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E109" s="28"/>
       <c r="F109" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G109" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="26">
         <v>96</v>
       </c>
       <c r="B110" s="27" t="s">
-        <v>239</v>
+        <v>19</v>
       </c>
       <c r="C110" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="D110" s="28"/>
+        <v>27</v>
+      </c>
+      <c r="D110" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E110" s="28"/>
       <c r="F110" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G110" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>97</v>
       </c>
       <c r="B111" s="27" t="s">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="D111" s="28"/>
+        <v>28</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E111" s="28"/>
       <c r="F111" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G111" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="26">
         <v>98</v>
       </c>
       <c r="B112" s="27" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="D112" s="28"/>
+        <v>30</v>
+      </c>
+      <c r="D112" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E112" s="28"/>
       <c r="F112" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G112" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>99</v>
       </c>
       <c r="B113" s="27" t="s">
-        <v>242</v>
+        <v>20</v>
       </c>
       <c r="C113" s="28" t="s">
-        <v>256</v>
-      </c>
-      <c r="D113" s="28"/>
+        <v>343</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E113" s="28"/>
       <c r="F113" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G113" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="26">
         <v>100</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>243</v>
+        <v>345</v>
       </c>
       <c r="C114" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="D114" s="28"/>
+        <v>344</v>
+      </c>
+      <c r="D114" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E114" s="28"/>
       <c r="F114" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G114" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
         <v>101</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>244</v>
+        <v>382</v>
       </c>
       <c r="C115" s="28" t="s">
-        <v>250</v>
+        <v>385</v>
       </c>
       <c r="D115" s="28"/>
       <c r="E115" s="28"/>
       <c r="F115" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G115" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>102</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>275</v>
+        <v>383</v>
       </c>
       <c r="C116" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="D116" s="28"/>
+        <v>384</v>
+      </c>
+      <c r="D116" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E116" s="28"/>
       <c r="F116" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G116" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="26">
         <v>103</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C117" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="D117" s="28"/>
+      <c r="D117" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E117" s="28"/>
       <c r="F117" s="29" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="G117" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>104</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="D118" s="28"/>
+        <v>266</v>
+      </c>
+      <c r="D118" s="28" t="s">
+        <v>48</v>
+      </c>
       <c r="E118" s="28"/>
       <c r="F118" s="29" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="G118" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
         <v>105</v>
       </c>
       <c r="B119" s="27" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="C119" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D119" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="D119" s="28"/>
       <c r="E119" s="28"/>
       <c r="F119" s="29" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="G119" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="26">
         <v>106</v>
       </c>
       <c r="B120" s="27" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="C120" s="28" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="D120" s="28"/>
       <c r="E120" s="28"/>
       <c r="F120" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G120" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>107</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="D121" s="28"/>
       <c r="E121" s="28"/>
       <c r="F121" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G121" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>108</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="D122" s="28"/>
       <c r="E122" s="28"/>
       <c r="F122" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G122" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="26">
         <v>109</v>
       </c>
       <c r="B123" s="27" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C123" s="28" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="D123" s="28"/>
       <c r="E123" s="28"/>
       <c r="F123" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G123" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>110</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="C124" s="28" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="D124" s="28"/>
       <c r="E124" s="28"/>
       <c r="F124" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G124" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>111</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="C125" s="28" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="D125" s="28"/>
       <c r="E125" s="28"/>
       <c r="F125" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G125" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="26">
         <v>112</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="C126" s="28" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D126" s="28"/>
       <c r="E126" s="28"/>
       <c r="F126" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G126" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
         <v>113</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="C127" s="28" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="D127" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E127" s="28"/>
       <c r="F127" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G127" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>114</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C128" s="28" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="D128" s="28"/>
       <c r="E128" s="28"/>
       <c r="F128" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G128" s="30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="26">
         <v>115</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C129" s="28" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D129" s="28"/>
       <c r="E129" s="28"/>
       <c r="F129" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G129" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>116</v>
+      </c>
+      <c r="B130" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C130" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G130" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>117</v>
+      </c>
+      <c r="B131" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C131" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="D131" s="28"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G131" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="26">
+        <v>118</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C132" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="D132" s="28"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G132" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>119</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C133" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="D133" s="28"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G133" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>120</v>
+      </c>
+      <c r="B134" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="D134" s="28"/>
+      <c r="E134" s="28"/>
+      <c r="F134" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G134" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="26">
+        <v>121</v>
+      </c>
+      <c r="B135" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="C135" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D135" s="28"/>
+      <c r="E135" s="28"/>
+      <c r="F135" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G135" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>122</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C136" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G136" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>123</v>
+      </c>
+      <c r="B137" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C137" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="D137" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E137" s="28"/>
+      <c r="F137" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G137" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="26">
+        <v>124</v>
+      </c>
+      <c r="B138" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C138" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="D138" s="28"/>
+      <c r="E138" s="28"/>
+      <c r="F138" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G138" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>125</v>
+      </c>
+      <c r="B139" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C139" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D139" s="28"/>
+      <c r="E139" s="28"/>
+      <c r="F139" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G139" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>126</v>
+      </c>
+      <c r="B140" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C140" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="D140" s="28"/>
+      <c r="E140" s="28"/>
+      <c r="F140" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G140" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="26">
+        <v>127</v>
+      </c>
+      <c r="B141" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
+      <c r="F141" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G141" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>128</v>
+      </c>
+      <c r="B142" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C142" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="D142" s="28"/>
+      <c r="E142" s="28"/>
+      <c r="F142" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G142" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>129</v>
+      </c>
+      <c r="B143" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C143" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D143" s="28"/>
+      <c r="E143" s="28"/>
+      <c r="F143" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G143" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="26">
+        <v>130</v>
+      </c>
+      <c r="B144" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="D144" s="28"/>
+      <c r="E144" s="28"/>
+      <c r="F144" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G144" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>131</v>
+      </c>
+      <c r="B145" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C145" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="D145" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E145" s="28"/>
+      <c r="F145" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G145" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>132</v>
+      </c>
+      <c r="B146" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D146" s="28"/>
+      <c r="E146" s="28"/>
+      <c r="F146" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G146" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="26">
+        <v>133</v>
+      </c>
+      <c r="B147" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C147" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D147" s="28"/>
+      <c r="E147" s="28"/>
+      <c r="F147" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G147" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>134</v>
+      </c>
+      <c r="B148" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="C148" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="D148" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E148" s="28"/>
+      <c r="F148" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G148" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>135</v>
+      </c>
+      <c r="B149" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="C149" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="D149" s="28"/>
+      <c r="E149" s="28"/>
+      <c r="F149" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G149" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="26">
+        <v>136</v>
+      </c>
+      <c r="B150" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="C150" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="D150" s="28"/>
+      <c r="E150" s="28"/>
+      <c r="F150" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G150" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>137</v>
+      </c>
+      <c r="B151" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="C151" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="D151" s="28"/>
+      <c r="E151" s="28"/>
+      <c r="F151" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G151" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>138</v>
+      </c>
+      <c r="B152" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="C152" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="D152" s="28"/>
+      <c r="E152" s="28"/>
+      <c r="F152" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G152" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="26">
+        <v>139</v>
+      </c>
+      <c r="B153" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="C153" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="D153" s="28"/>
+      <c r="E153" s="28"/>
+      <c r="F153" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G153" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>140</v>
+      </c>
+      <c r="B154" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="C154" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="D154" s="28"/>
+      <c r="E154" s="28"/>
+      <c r="F154" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G154" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>141</v>
+      </c>
+      <c r="B155" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="C155" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="D155" s="28"/>
+      <c r="E155" s="28"/>
+      <c r="F155" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G155" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="26">
+        <v>142</v>
+      </c>
+      <c r="B156" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="C156" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="D156" s="28"/>
+      <c r="E156" s="28"/>
+      <c r="F156" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="G156" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>143</v>
+      </c>
+      <c r="B157" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="C157" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="D157" s="28"/>
+      <c r="E157" s="28"/>
+      <c r="F157" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G157" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>144</v>
+      </c>
+      <c r="B158" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="C158" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="D158" s="28"/>
+      <c r="E158" s="28"/>
+      <c r="F158" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G158" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="26">
+        <v>145</v>
+      </c>
+      <c r="B159" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="C159" s="28" t="s">
+        <v>392</v>
+      </c>
+      <c r="D159" s="28"/>
+      <c r="E159" s="28"/>
+      <c r="F159" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G159" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>146</v>
+      </c>
+      <c r="B160" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="C160" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="D160" s="28"/>
+      <c r="E160" s="28"/>
+      <c r="F160" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G160" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>147</v>
+      </c>
+      <c r="B161" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="C161" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="D161" s="28"/>
+      <c r="E161" s="28"/>
+      <c r="F161" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G161" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="26">
+        <v>148</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="C162" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="D162" s="28"/>
+      <c r="E162" s="28"/>
+      <c r="F162" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G162" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>149</v>
+      </c>
+      <c r="B163" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="C163" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="D163" s="28"/>
+      <c r="E163" s="28"/>
+      <c r="F163" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G163" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>150</v>
+      </c>
+      <c r="B164" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="C164" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D164" s="28"/>
+      <c r="E164" s="28"/>
+      <c r="F164" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G164" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="26">
+        <v>151</v>
+      </c>
+      <c r="B165" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="C165" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="D165" s="28"/>
+      <c r="E165" s="28"/>
+      <c r="F165" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="G165" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>152</v>
+      </c>
+      <c r="B166" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="C166" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="D166" s="28"/>
+      <c r="E166" s="28"/>
+      <c r="F166" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G166" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>153</v>
+      </c>
+      <c r="B167" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="C167" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="D167" s="28"/>
+      <c r="E167" s="28"/>
+      <c r="F167" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G167" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="26">
+        <v>154</v>
+      </c>
+      <c r="B168" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="C168" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="D168" s="28"/>
+      <c r="E168" s="28"/>
+      <c r="F168" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G168" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>155</v>
+      </c>
+      <c r="B169" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="C169" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="D169" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E169" s="28"/>
+      <c r="F169" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G169" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>156</v>
+      </c>
+      <c r="B170" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="C170" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="D170" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E170" s="28"/>
+      <c r="F170" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G170" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="26">
+        <v>157</v>
+      </c>
+      <c r="B171" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="C171" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="D171" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E171" s="28"/>
+      <c r="F171" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G171" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>158</v>
+      </c>
+      <c r="B172" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="C172" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="D172" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E172" s="28"/>
+      <c r="F172" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G172" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>159</v>
+      </c>
+      <c r="B173" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="C173" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="D173" s="28"/>
+      <c r="E173" s="28"/>
+      <c r="F173" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G173" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="26">
+        <v>160</v>
+      </c>
+      <c r="B174" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="C174" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="D174" s="28"/>
+      <c r="E174" s="28"/>
+      <c r="F174" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G174" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>161</v>
+      </c>
+      <c r="B175" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="C175" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="D175" s="28"/>
+      <c r="E175" s="28"/>
+      <c r="F175" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G175" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>162</v>
+      </c>
+      <c r="B176" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="C176" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="D176" s="28"/>
+      <c r="E176" s="28"/>
+      <c r="F176" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G176" s="30" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B61:F65">
+    <sortCondition ref="B61:B65"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0">

</xml_diff>

<commit_message>
XLAM decompiliert, Ribbon-Pointer gelöscht, schreibgeschützt
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C251C1-4A2C-479A-B57A-B5DB8BAF67F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10" yWindow="3290" windowWidth="15340" windowHeight="6230" activeTab="1"/>
+    <workbookView xWindow="3480" yWindow="2080" windowWidth="19000" windowHeight="11970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
@@ -29,12 +35,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Robert Schwenn</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -108,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -148,12 +154,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Robert Schwenn</author>
   </authors>
   <commentList>
-    <comment ref="A13" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -210,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -261,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -276,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -291,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -306,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -808,13 +814,7 @@
     <t>Anwender</t>
   </si>
   <si>
-    <t>... zwecks Anpassungen für Ermittlung der Projektdaten und Liste der speziellen ASCII-Formate.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Die gefilterte Liste enthält nur solche Zielformate, die wenigstens eine der Kategorien der Quelldatei aufweist.</t>
-  </si>
-  <si>
-    <t>intermetric</t>
   </si>
   <si>
     <t>TK.QKm</t>
@@ -1672,11 +1672,17 @@
   <si>
     <t>LRP AnschriebTyp</t>
   </si>
+  <si>
+    <t>nicht mehr verwendet</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2253,6 +2259,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2274,7 +2283,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="18433" name="Group 1"/>
+        <xdr:cNvPr id="18433" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks noChangeAspect="1"/>
         </xdr:cNvGrpSpPr>
@@ -2289,7 +2304,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="18434" name="Rectangle 2"/>
+          <xdr:cNvPr id="18434" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002480000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -2331,11 +2352,14 @@
                   <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                     <a14:compatExt spid="_x0000_s18435"/>
                   </a:ext>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003480000}"/>
+                  </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
-            <xdr:spPr>
+            <xdr:spPr bwMode="auto">
               <a:xfrm>
                 <a:off x="9766300" y="0"/>
                 <a:ext cx="0" cy="0"/>
@@ -2343,6 +2367,29 @@
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:extLst>
+                <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                  <a14:hiddenFill>
+                    <a:solidFill>
+                      <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    </a:solidFill>
+                  </a14:hiddenFill>
+                </a:ext>
+                <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                  <a14:hiddenLine w="1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    </a:solidFill>
+                    <a:miter lim="800000"/>
+                    <a:headEnd/>
+                    <a:tailEnd/>
+                  </a14:hiddenLine>
+                </a:ext>
+              </a:extLst>
             </xdr:spPr>
           </xdr:sp>
         </mc:Choice>
@@ -2366,7 +2413,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18436" name="Line 4"/>
+        <xdr:cNvPr id="18436" name="Line 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2414,7 +2467,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18437" name="Line 5"/>
+        <xdr:cNvPr id="18437" name="Line 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2462,7 +2521,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18438" name="Line 6"/>
+        <xdr:cNvPr id="18438" name="Line 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2510,7 +2575,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18439" name="Line 7"/>
+        <xdr:cNvPr id="18439" name="Line 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2558,7 +2629,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18440" name="Line 8"/>
+        <xdr:cNvPr id="18440" name="Line 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2606,7 +2683,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18441" name="Line 9"/>
+        <xdr:cNvPr id="18441" name="Line 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2654,7 +2737,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18442" name="Line 10"/>
+        <xdr:cNvPr id="18442" name="Line 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2702,7 +2791,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18443" name="Line 11"/>
+        <xdr:cNvPr id="18443" name="Line 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2750,7 +2845,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18444" name="Line 12"/>
+        <xdr:cNvPr id="18444" name="Line 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2798,7 +2899,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18445" name="Line 13"/>
+        <xdr:cNvPr id="18445" name="Line 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2846,7 +2953,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18446" name="Line 14"/>
+        <xdr:cNvPr id="18446" name="Line 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2894,7 +3007,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18447" name="Line 15"/>
+        <xdr:cNvPr id="18447" name="Line 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2942,7 +3061,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18448" name="Line 16"/>
+        <xdr:cNvPr id="18448" name="Line 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -2990,7 +3115,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18449" name="Line 17"/>
+        <xdr:cNvPr id="18449" name="Line 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -3038,7 +3169,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18450" name="Line 18"/>
+        <xdr:cNvPr id="18450" name="Line 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012480000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -3445,7 +3582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="tabEinstellungen">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3454,7 +3591,7 @@
     <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3494,10 +3631,10 @@
         <v>159</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>162</v>
+        <v>413</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>160</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3524,13 +3661,13 @@
     </row>
     <row r="7" spans="1:3" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3585,29 +3722,29 @@
         <v>152</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>154</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3626,14 +3763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3650,7 +3787,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="52" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -3662,7 +3799,7 @@
     <row r="2" spans="1:7" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
       <c r="B2" s="28" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="28"/>
@@ -3684,7 +3821,7 @@
     <row r="4" spans="1:7" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="28"/>
@@ -3695,7 +3832,7 @@
     <row r="5" spans="1:7" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32"/>
       <c r="B5" s="33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="35"/>
@@ -3706,7 +3843,7 @@
     <row r="6" spans="1:7" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
       <c r="B6" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="35"/>
@@ -3728,7 +3865,7 @@
     <row r="8" spans="1:7" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="33" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="35"/>
@@ -3739,7 +3876,7 @@
     <row r="9" spans="1:7" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="28"/>
@@ -3750,7 +3887,7 @@
     <row r="10" spans="1:7" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="28"/>
@@ -3761,7 +3898,7 @@
     <row r="11" spans="1:7" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="35"/>
@@ -3855,10 +3992,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -3872,10 +4009,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -3889,10 +4026,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -3906,10 +4043,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -3923,10 +4060,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -3940,10 +4077,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -3957,10 +4094,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -3974,10 +4111,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -4148,10 +4285,10 @@
         <v>20</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -4165,10 +4302,10 @@
         <v>21</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -4267,10 +4404,10 @@
         <v>27</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -4284,10 +4421,10 @@
         <v>28</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
@@ -4301,10 +4438,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -4318,10 +4455,10 @@
         <v>30</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -4335,10 +4472,10 @@
         <v>31</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
@@ -4352,10 +4489,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
@@ -4369,10 +4506,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -4386,10 +4523,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
@@ -4403,10 +4540,10 @@
         <v>35</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
@@ -4420,10 +4557,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
@@ -4445,7 +4582,7 @@
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G51" s="16" t="s">
         <v>61</v>
@@ -4464,7 +4601,7 @@
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
       <c r="F52" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G52" s="16" t="s">
         <v>61</v>
@@ -4483,7 +4620,7 @@
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>61</v>
@@ -4502,7 +4639,7 @@
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>61</v>
@@ -4521,7 +4658,7 @@
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>61</v>
@@ -4540,7 +4677,7 @@
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>61</v>
@@ -4559,7 +4696,7 @@
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G57" s="16" t="s">
         <v>61</v>
@@ -4578,7 +4715,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>61</v>
@@ -4597,7 +4734,7 @@
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>61</v>
@@ -4608,15 +4745,15 @@
         <v>46</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>61</v>
@@ -4627,15 +4764,15 @@
         <v>47</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>61</v>
@@ -4646,15 +4783,15 @@
         <v>48</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>61</v>
@@ -4665,7 +4802,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>88</v>
@@ -4673,7 +4810,7 @@
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
       <c r="F63" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>61</v>
@@ -4684,7 +4821,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>87</v>
@@ -4692,7 +4829,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>61</v>
@@ -4703,15 +4840,15 @@
         <v>51</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
       <c r="F65" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>61</v>
@@ -4785,10 +4922,10 @@
         <v>55</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>48</v>
@@ -4913,10 +5050,10 @@
         <v>61</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75" s="15"/>
@@ -4932,10 +5069,10 @@
         <v>62</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76" s="15"/>
@@ -4974,10 +5111,10 @@
         <v>64</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
@@ -5014,10 +5151,10 @@
         <v>66</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>48</v>
@@ -5077,10 +5214,10 @@
         <v>69</v>
       </c>
       <c r="B83" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>48</v>
@@ -5098,10 +5235,10 @@
         <v>70</v>
       </c>
       <c r="B84" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C84" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>276</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>48</v>
@@ -5119,10 +5256,10 @@
         <v>71</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>48</v>
@@ -5140,10 +5277,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D86" s="15" t="s">
         <v>48</v>
@@ -5161,10 +5298,10 @@
         <v>73</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>48</v>
@@ -5182,10 +5319,10 @@
         <v>74</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D88" s="15" t="s">
         <v>48</v>
@@ -5531,10 +5668,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
@@ -5550,10 +5687,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D106" s="15"/>
       <c r="E106" s="15"/>
@@ -5569,10 +5706,10 @@
         <v>93</v>
       </c>
       <c r="B107" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C107" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="D107" s="15"/>
       <c r="E107" s="15"/>
@@ -5588,10 +5725,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D108" s="15"/>
       <c r="E108" s="15"/>
@@ -5694,7 +5831,7 @@
         <v>20</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>48</v>
@@ -5712,10 +5849,10 @@
         <v>100</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>48</v>
@@ -5733,10 +5870,10 @@
         <v>101</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D115" s="15"/>
       <c r="E115" s="15"/>
@@ -5752,10 +5889,10 @@
         <v>102</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>48</v>
@@ -5773,10 +5910,10 @@
         <v>103</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>48</v>
@@ -5794,10 +5931,10 @@
         <v>104</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>48</v>
@@ -5815,17 +5952,17 @@
         <v>105</v>
       </c>
       <c r="B119" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C119" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E119" s="15"/>
       <c r="F119" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G119" s="16" t="s">
         <v>61</v>
@@ -5836,17 +5973,17 @@
         <v>106</v>
       </c>
       <c r="B120" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C120" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>261</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E120" s="15"/>
       <c r="F120" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G120" s="16" t="s">
         <v>61</v>
@@ -5857,15 +5994,15 @@
         <v>107</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D121" s="15"/>
       <c r="E121" s="15"/>
       <c r="F121" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G121" s="16" t="s">
         <v>61</v>
@@ -5876,15 +6013,15 @@
         <v>108</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G122" s="16" t="s">
         <v>61</v>
@@ -5895,15 +6032,15 @@
         <v>109</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D123" s="15"/>
       <c r="E123" s="15"/>
       <c r="F123" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G123" s="16" t="s">
         <v>61</v>
@@ -5914,15 +6051,15 @@
         <v>110</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="15"/>
       <c r="F124" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G124" s="16" t="s">
         <v>61</v>
@@ -5933,15 +6070,15 @@
         <v>111</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D125" s="15"/>
       <c r="E125" s="15"/>
       <c r="F125" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G125" s="16" t="s">
         <v>61</v>
@@ -5952,15 +6089,15 @@
         <v>112</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D126" s="15"/>
       <c r="E126" s="15"/>
       <c r="F126" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G126" s="16" t="s">
         <v>61</v>
@@ -5971,15 +6108,15 @@
         <v>113</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D127" s="15"/>
       <c r="E127" s="15"/>
       <c r="F127" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G127" s="16" t="s">
         <v>61</v>
@@ -5990,15 +6127,15 @@
         <v>114</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="15"/>
       <c r="F128" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G128" s="16" t="s">
         <v>61</v>
@@ -6009,17 +6146,17 @@
         <v>115</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D129" s="15" t="s">
         <v>49</v>
       </c>
       <c r="E129" s="15"/>
       <c r="F129" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G129" s="16" t="s">
         <v>61</v>
@@ -6030,15 +6167,15 @@
         <v>116</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D130" s="15"/>
       <c r="E130" s="15"/>
       <c r="F130" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G130" s="16" t="s">
         <v>61</v>
@@ -6049,15 +6186,15 @@
         <v>117</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="15"/>
       <c r="F131" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G131" s="16" t="s">
         <v>61</v>
@@ -6068,15 +6205,15 @@
         <v>118</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="15"/>
       <c r="F132" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G132" s="16" t="s">
         <v>61</v>
@@ -6087,15 +6224,15 @@
         <v>119</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="15"/>
       <c r="F133" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G133" s="16" t="s">
         <v>61</v>
@@ -6106,15 +6243,15 @@
         <v>120</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="15"/>
       <c r="F134" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G134" s="16" t="s">
         <v>61</v>
@@ -6125,15 +6262,15 @@
         <v>121</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="15"/>
       <c r="F135" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G135" s="16" t="s">
         <v>61</v>
@@ -6144,15 +6281,15 @@
         <v>122</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
       <c r="F136" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G136" s="16" t="s">
         <v>61</v>
@@ -6163,15 +6300,15 @@
         <v>123</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="15"/>
       <c r="F137" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G137" s="16" t="s">
         <v>61</v>
@@ -6182,15 +6319,15 @@
         <v>124</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="15"/>
       <c r="F138" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G138" s="16" t="s">
         <v>61</v>
@@ -6201,17 +6338,17 @@
         <v>125</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D139" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E139" s="15"/>
       <c r="F139" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G139" s="16" t="s">
         <v>61</v>
@@ -6222,15 +6359,15 @@
         <v>126</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D140" s="15"/>
       <c r="E140" s="15"/>
       <c r="F140" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G140" s="16" t="s">
         <v>61</v>
@@ -6241,15 +6378,15 @@
         <v>127</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="15"/>
       <c r="F141" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G141" s="16" t="s">
         <v>61</v>
@@ -6260,15 +6397,15 @@
         <v>128</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="15"/>
       <c r="F142" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G142" s="16" t="s">
         <v>61</v>
@@ -6279,15 +6416,15 @@
         <v>129</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="15"/>
       <c r="F143" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G143" s="16" t="s">
         <v>61</v>
@@ -6298,15 +6435,15 @@
         <v>130</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="15"/>
       <c r="F144" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G144" s="16" t="s">
         <v>61</v>
@@ -6317,15 +6454,15 @@
         <v>131</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="15"/>
       <c r="F145" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G145" s="16" t="s">
         <v>61</v>
@@ -6336,15 +6473,15 @@
         <v>132</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="15"/>
       <c r="F146" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G146" s="16" t="s">
         <v>61</v>
@@ -6355,17 +6492,17 @@
         <v>133</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D147" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E147" s="15"/>
       <c r="F147" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G147" s="16" t="s">
         <v>61</v>
@@ -6376,15 +6513,15 @@
         <v>134</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="15"/>
       <c r="F148" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G148" s="16" t="s">
         <v>61</v>
@@ -6395,15 +6532,15 @@
         <v>135</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="15"/>
       <c r="F149" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G149" s="16" t="s">
         <v>61</v>
@@ -6414,17 +6551,17 @@
         <v>136</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D150" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E150" s="15"/>
       <c r="F150" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G150" s="16" t="s">
         <v>61</v>
@@ -6435,15 +6572,15 @@
         <v>137</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D151" s="15"/>
       <c r="E151" s="15"/>
       <c r="F151" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G151" s="16" t="s">
         <v>61</v>
@@ -6454,15 +6591,15 @@
         <v>138</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="15"/>
       <c r="F152" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G152" s="16" t="s">
         <v>61</v>
@@ -6473,15 +6610,15 @@
         <v>139</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
       <c r="F153" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G153" s="16" t="s">
         <v>61</v>
@@ -6492,15 +6629,15 @@
         <v>140</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="15"/>
       <c r="F154" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G154" s="16" t="s">
         <v>61</v>
@@ -6511,15 +6648,15 @@
         <v>141</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="15"/>
       <c r="F155" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G155" s="16" t="s">
         <v>61</v>
@@ -6530,15 +6667,15 @@
         <v>142</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="15"/>
       <c r="F156" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G156" s="16" t="s">
         <v>61</v>
@@ -6549,15 +6686,15 @@
         <v>143</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
       <c r="F157" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G157" s="16" t="s">
         <v>61</v>
@@ -6568,15 +6705,15 @@
         <v>144</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="15"/>
       <c r="F158" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G158" s="16" t="s">
         <v>61</v>
@@ -6587,15 +6724,15 @@
         <v>145</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="15"/>
       <c r="F159" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G159" s="16" t="s">
         <v>61</v>
@@ -6606,15 +6743,15 @@
         <v>146</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
       <c r="F160" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G160" s="16" t="s">
         <v>61</v>
@@ -6625,15 +6762,15 @@
         <v>147</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="15"/>
       <c r="F161" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G161" s="16" t="s">
         <v>61</v>
@@ -6644,15 +6781,15 @@
         <v>148</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
       <c r="F162" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G162" s="16" t="s">
         <v>61</v>
@@ -6663,15 +6800,15 @@
         <v>149</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="15"/>
       <c r="F163" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G163" s="16" t="s">
         <v>61</v>
@@ -6682,15 +6819,15 @@
         <v>150</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
       <c r="F164" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G164" s="16" t="s">
         <v>61</v>
@@ -6701,15 +6838,15 @@
         <v>151</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
       <c r="F165" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G165" s="16" t="s">
         <v>61</v>
@@ -6720,15 +6857,15 @@
         <v>152</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
       <c r="F166" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G166" s="16" t="s">
         <v>61</v>
@@ -6739,15 +6876,15 @@
         <v>153</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D167" s="15"/>
       <c r="E167" s="15"/>
       <c r="F167" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G167" s="16" t="s">
         <v>61</v>
@@ -6758,15 +6895,15 @@
         <v>154</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D168" s="15"/>
       <c r="E168" s="15"/>
       <c r="F168" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G168" s="16" t="s">
         <v>61</v>
@@ -6777,15 +6914,15 @@
         <v>155</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D169" s="15"/>
       <c r="E169" s="15"/>
       <c r="F169" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G169" s="16" t="s">
         <v>61</v>
@@ -6796,15 +6933,15 @@
         <v>156</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
       <c r="F170" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G170" s="16" t="s">
         <v>61</v>
@@ -6815,17 +6952,17 @@
         <v>157</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D171" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E171" s="15"/>
       <c r="F171" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G171" s="16" t="s">
         <v>61</v>
@@ -6836,17 +6973,17 @@
         <v>158</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E172" s="15"/>
       <c r="F172" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G172" s="16" t="s">
         <v>61</v>
@@ -6857,17 +6994,17 @@
         <v>159</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E173" s="15"/>
       <c r="F173" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G173" s="16" t="s">
         <v>61</v>
@@ -6878,17 +7015,17 @@
         <v>160</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E174" s="15"/>
       <c r="F174" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G174" s="16" t="s">
         <v>61</v>
@@ -6899,15 +7036,15 @@
         <v>161</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="15"/>
       <c r="F175" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G175" s="16" t="s">
         <v>61</v>
@@ -6918,15 +7055,15 @@
         <v>162</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="15"/>
       <c r="F176" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G176" s="16" t="s">
         <v>61</v>
@@ -6937,15 +7074,15 @@
         <v>163</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
       <c r="F177" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G177" s="16" t="s">
         <v>61</v>
@@ -6956,15 +7093,15 @@
         <v>164</v>
       </c>
       <c r="B178" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="C178" s="15" t="s">
         <v>381</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>383</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
       <c r="F178" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G178" s="16" t="s">
         <v>61</v>
@@ -6975,15 +7112,15 @@
         <v>165</v>
       </c>
       <c r="B179" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C179" s="15" t="s">
         <v>382</v>
-      </c>
-      <c r="C179" s="15" t="s">
-        <v>384</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
       <c r="F179" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G179" s="16" t="s">
         <v>61</v>
@@ -6994,15 +7131,15 @@
         <v>166</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
       <c r="F180" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G180" s="16" t="s">
         <v>61</v>
@@ -7013,15 +7150,15 @@
         <v>167</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
       <c r="F181" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G181" s="16" t="s">
         <v>61</v>
@@ -7032,15 +7169,15 @@
         <v>168</v>
       </c>
       <c r="B182" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C182" s="15" t="s">
         <v>398</v>
-      </c>
-      <c r="C182" s="15" t="s">
-        <v>400</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
       <c r="F182" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G182" s="16" t="s">
         <v>61</v>
@@ -7051,15 +7188,15 @@
         <v>169</v>
       </c>
       <c r="B183" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C183" s="15" t="s">
         <v>399</v>
-      </c>
-      <c r="C183" s="15" t="s">
-        <v>401</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
       <c r="F183" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G183" s="16" t="s">
         <v>61</v>
@@ -7070,15 +7207,15 @@
         <v>170</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15"/>
       <c r="F184" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G184" s="16" t="s">
         <v>61</v>
@@ -7089,15 +7226,15 @@
         <v>171</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
       <c r="F185" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G185" s="16" t="s">
         <v>61</v>
@@ -7108,22 +7245,22 @@
         <v>172</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
       <c r="F186" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G186" s="16" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B61:F65">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B61:F65">
     <sortCondition ref="B61:B65"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>

<commit_message>
CimpTrassenkoo A0: Unterstützung für Gradientenneigung
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35C251C1-4A2C-479A-B57A-B5DB8BAF67F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7D66138-4929-42FE-A751-2E116723A1F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2080" windowWidth="19000" windowHeight="11970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2770" yWindow="1400" windowWidth="18170" windowHeight="11100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$115</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -332,7 +332,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="416">
   <si>
     <t>GK.X</t>
   </si>
@@ -1677,6 +1677,12 @@
   </si>
   <si>
     <t>dummy</t>
+  </si>
+  <si>
+    <t>Tra.G</t>
+  </si>
+  <si>
+    <t>Steigungswinkel der Gradiente</t>
   </si>
 </sst>
 </file>
@@ -3767,10 +3773,10 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5803,14 +5809,14 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="11">
+      <c r="A112" s="1">
         <v>98</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>18</v>
+        <v>414</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>30</v>
+        <v>415</v>
       </c>
       <c r="D112" s="15" t="s">
         <v>49</v>
@@ -5824,17 +5830,17 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="1">
+      <c r="A113" s="11">
         <v>99</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>336</v>
+        <v>30</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E113" s="15"/>
       <c r="F113" s="15" t="s">
@@ -5845,14 +5851,14 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="11">
+      <c r="A114" s="1">
         <v>100</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>338</v>
+        <v>20</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>48</v>
@@ -5870,12 +5876,14 @@
         <v>101</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>375</v>
+        <v>338</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D115" s="15"/>
+        <v>337</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E115" s="15"/>
       <c r="F115" s="15" t="s">
         <v>25</v>
@@ -5885,18 +5893,16 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="1">
+      <c r="A116" s="11">
         <v>102</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="D116" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="D116" s="15"/>
       <c r="E116" s="15"/>
       <c r="F116" s="15" t="s">
         <v>25</v>
@@ -5906,14 +5912,14 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="11">
+      <c r="A117" s="1">
         <v>103</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D117" s="15" t="s">
         <v>48</v>
@@ -5931,10 +5937,10 @@
         <v>104</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>48</v>
@@ -5948,35 +5954,35 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="1">
+      <c r="A119" s="11">
         <v>105</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>256</v>
+        <v>376</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>258</v>
+        <v>377</v>
       </c>
       <c r="D119" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E119" s="15"/>
       <c r="F119" s="15" t="s">
-        <v>260</v>
+        <v>25</v>
       </c>
       <c r="G119" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="11">
+      <c r="A120" s="1">
         <v>106</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D120" s="15" t="s">
         <v>48</v>
@@ -5994,12 +6000,14 @@
         <v>107</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D121" s="15"/>
+        <v>259</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E121" s="15"/>
       <c r="F121" s="15" t="s">
         <v>260</v>
@@ -6009,33 +6017,33 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="1">
+      <c r="A122" s="11">
         <v>108</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="15" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="G122" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="11">
+      <c r="A123" s="1">
         <v>109</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D123" s="15"/>
       <c r="E123" s="15"/>
@@ -6051,10 +6059,10 @@
         <v>110</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="15"/>
@@ -6066,14 +6074,14 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="1">
+      <c r="A125" s="11">
         <v>111</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D125" s="15"/>
       <c r="E125" s="15"/>
@@ -6085,14 +6093,14 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="11">
+      <c r="A126" s="1">
         <v>112</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="D126" s="15"/>
       <c r="E126" s="15"/>
@@ -6108,10 +6116,10 @@
         <v>113</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D127" s="15"/>
       <c r="E127" s="15"/>
@@ -6123,14 +6131,14 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="1">
+      <c r="A128" s="11">
         <v>114</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D128" s="15"/>
       <c r="E128" s="15"/>
@@ -6142,18 +6150,16 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="11">
+      <c r="A129" s="1">
         <v>115</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="D129" s="15" t="s">
-        <v>49</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="D129" s="15"/>
       <c r="E129" s="15"/>
       <c r="F129" s="15" t="s">
         <v>224</v>
@@ -6167,12 +6173,14 @@
         <v>116</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="D130" s="15"/>
+        <v>221</v>
+      </c>
+      <c r="D130" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="E130" s="15"/>
       <c r="F130" s="15" t="s">
         <v>224</v>
@@ -6182,14 +6190,14 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="1">
+      <c r="A131" s="11">
         <v>117</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="D131" s="15"/>
       <c r="E131" s="15"/>
@@ -6201,14 +6209,14 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="11">
+      <c r="A132" s="1">
         <v>118</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="D132" s="15"/>
       <c r="E132" s="15"/>
@@ -6224,10 +6232,10 @@
         <v>119</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D133" s="15"/>
       <c r="E133" s="15"/>
@@ -6239,14 +6247,14 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="1">
+      <c r="A134" s="11">
         <v>120</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D134" s="15"/>
       <c r="E134" s="15"/>
@@ -6258,14 +6266,14 @@
       </c>
     </row>
     <row r="135" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="11">
+      <c r="A135" s="1">
         <v>121</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D135" s="15"/>
       <c r="E135" s="15"/>
@@ -6281,10 +6289,10 @@
         <v>122</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
@@ -6296,14 +6304,14 @@
       </c>
     </row>
     <row r="137" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="1">
+      <c r="A137" s="11">
         <v>123</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="15"/>
@@ -6315,14 +6323,14 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="11">
+      <c r="A138" s="1">
         <v>124</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="15"/>
@@ -6338,14 +6346,12 @@
         <v>125</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="D139" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D139" s="15"/>
       <c r="E139" s="15"/>
       <c r="F139" s="15" t="s">
         <v>224</v>
@@ -6355,16 +6361,18 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="1">
+      <c r="A140" s="11">
         <v>126</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D140" s="15"/>
+        <v>239</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E140" s="15"/>
       <c r="F140" s="15" t="s">
         <v>224</v>
@@ -6374,14 +6382,14 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="11">
+      <c r="A141" s="1">
         <v>127</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D141" s="15"/>
       <c r="E141" s="15"/>
@@ -6397,10 +6405,10 @@
         <v>128</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D142" s="15"/>
       <c r="E142" s="15"/>
@@ -6412,14 +6420,14 @@
       </c>
     </row>
     <row r="143" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="1">
+      <c r="A143" s="11">
         <v>129</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="D143" s="15"/>
       <c r="E143" s="15"/>
@@ -6431,14 +6439,14 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="11">
+      <c r="A144" s="1">
         <v>130</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="D144" s="15"/>
       <c r="E144" s="15"/>
@@ -6454,10 +6462,10 @@
         <v>131</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="D145" s="15"/>
       <c r="E145" s="15"/>
@@ -6469,37 +6477,35 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="1">
+      <c r="A146" s="11">
         <v>132</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>195</v>
+        <v>242</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="15"/>
       <c r="F146" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G146" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="11">
+      <c r="A147" s="1">
         <v>133</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D147" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="D147" s="15"/>
       <c r="E147" s="15"/>
       <c r="F147" s="15" t="s">
         <v>223</v>
@@ -6513,12 +6519,14 @@
         <v>134</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D148" s="15"/>
+        <v>199</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E148" s="15"/>
       <c r="F148" s="15" t="s">
         <v>223</v>
@@ -6528,14 +6536,14 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="1">
+      <c r="A149" s="11">
         <v>135</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D149" s="15"/>
       <c r="E149" s="15"/>
@@ -6547,18 +6555,16 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="11">
+      <c r="A150" s="1">
         <v>136</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>307</v>
+        <v>192</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="D150" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="D150" s="15"/>
       <c r="E150" s="15"/>
       <c r="F150" s="15" t="s">
         <v>223</v>
@@ -6572,29 +6578,31 @@
         <v>137</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="D151" s="15"/>
+        <v>308</v>
+      </c>
+      <c r="D151" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E151" s="15"/>
       <c r="F151" s="15" t="s">
-        <v>319</v>
+        <v>223</v>
       </c>
       <c r="G151" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="1">
+      <c r="A152" s="11">
         <v>138</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="15"/>
@@ -6606,14 +6614,14 @@
       </c>
     </row>
     <row r="153" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="11">
+      <c r="A153" s="1">
         <v>139</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
@@ -6629,10 +6637,10 @@
         <v>140</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="15"/>
@@ -6644,14 +6652,14 @@
       </c>
     </row>
     <row r="155" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="1">
+      <c r="A155" s="11">
         <v>141</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="15"/>
@@ -6663,14 +6671,14 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="11">
+      <c r="A156" s="1">
         <v>142</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C156" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="15"/>
@@ -6686,10 +6694,10 @@
         <v>143</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C157" s="15" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
@@ -6701,14 +6709,14 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="1">
+      <c r="A158" s="11">
         <v>144</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C158" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="15"/>
@@ -6720,19 +6728,19 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="11">
+      <c r="A159" s="1">
         <v>145</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="C159" s="15" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="15"/>
       <c r="F159" s="15" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="G159" s="16" t="s">
         <v>61</v>
@@ -6743,10 +6751,10 @@
         <v>146</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
       <c r="C160" s="15" t="s">
-        <v>384</v>
+        <v>345</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
@@ -6758,14 +6766,14 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="1">
+      <c r="A161" s="11">
         <v>147</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C161" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="15"/>
@@ -6777,14 +6785,14 @@
       </c>
     </row>
     <row r="162" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="11">
+      <c r="A162" s="1">
         <v>148</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>346</v>
+        <v>386</v>
       </c>
       <c r="C162" s="15" t="s">
-        <v>343</v>
+        <v>385</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
@@ -6800,10 +6808,10 @@
         <v>149</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="15"/>
@@ -6815,14 +6823,14 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="1">
+      <c r="A164" s="11">
         <v>150</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
@@ -6834,14 +6842,14 @@
       </c>
     </row>
     <row r="165" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="11">
+      <c r="A165" s="1">
         <v>151</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
@@ -6857,10 +6865,10 @@
         <v>152</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C166" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
@@ -6872,14 +6880,14 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="1">
+      <c r="A167" s="11">
         <v>153</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C167" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D167" s="15"/>
       <c r="E167" s="15"/>
@@ -6891,19 +6899,19 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="11">
+      <c r="A168" s="1">
         <v>154</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C168" s="15" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D168" s="15"/>
       <c r="E168" s="15"/>
       <c r="F168" s="15" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G168" s="16" t="s">
         <v>61</v>
@@ -6914,10 +6922,10 @@
         <v>155</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C169" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D169" s="15"/>
       <c r="E169" s="15"/>
@@ -6929,14 +6937,14 @@
       </c>
     </row>
     <row r="170" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="1">
+      <c r="A170" s="11">
         <v>156</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C170" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
@@ -6948,18 +6956,16 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="11">
+      <c r="A171" s="1">
         <v>157</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="D171" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="D171" s="15"/>
       <c r="E171" s="15"/>
       <c r="F171" s="15" t="s">
         <v>341</v>
@@ -6973,10 +6979,10 @@
         <v>158</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="C172" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D172" s="15" t="s">
         <v>48</v>
@@ -6990,14 +6996,14 @@
       </c>
     </row>
     <row r="173" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="1">
+      <c r="A173" s="11">
         <v>159</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C173" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>48</v>
@@ -7011,14 +7017,14 @@
       </c>
     </row>
     <row r="174" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="11">
+      <c r="A174" s="1">
         <v>160</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C174" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D174" s="15" t="s">
         <v>48</v>
@@ -7036,12 +7042,14 @@
         <v>161</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C175" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="D175" s="15"/>
+        <v>367</v>
+      </c>
+      <c r="D175" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E175" s="15"/>
       <c r="F175" s="15" t="s">
         <v>341</v>
@@ -7051,14 +7059,14 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="1">
+      <c r="A176" s="11">
         <v>162</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C176" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="15"/>
@@ -7070,14 +7078,14 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="11">
+      <c r="A177" s="1">
         <v>163</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>406</v>
+        <v>374</v>
       </c>
       <c r="C177" s="15" t="s">
-        <v>407</v>
+        <v>368</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
@@ -7093,10 +7101,10 @@
         <v>164</v>
       </c>
       <c r="B178" s="14" t="s">
-        <v>379</v>
+        <v>406</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
@@ -7108,14 +7116,14 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="1">
+      <c r="A179" s="11">
         <v>165</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
@@ -7127,14 +7135,14 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="11">
+      <c r="A180" s="1">
         <v>166</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
@@ -7150,10 +7158,10 @@
         <v>167</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C181" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
@@ -7165,14 +7173,14 @@
       </c>
     </row>
     <row r="182" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="1">
+      <c r="A182" s="11">
         <v>168</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C182" s="15" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
@@ -7184,14 +7192,14 @@
       </c>
     </row>
     <row r="183" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="11">
+      <c r="A183" s="1">
         <v>169</v>
       </c>
       <c r="B183" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C183" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
@@ -7207,10 +7215,10 @@
         <v>170</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C184" s="15" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15"/>
@@ -7222,14 +7230,14 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="1">
+      <c r="A185" s="11">
         <v>171</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
@@ -7241,14 +7249,14 @@
       </c>
     </row>
     <row r="186" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="11">
+      <c r="A186" s="1">
         <v>172</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
@@ -7256,6 +7264,25 @@
         <v>341</v>
       </c>
       <c r="G186" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A187" s="1">
+        <v>173</v>
+      </c>
+      <c r="B187" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="C187" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D187" s="15"/>
+      <c r="E187" s="15"/>
+      <c r="F187" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G187" s="16" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GeoTools_cfg.xlsx: Zuordnung der iGeo-A0-Felder dokumentiert
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26A62E4-F083-4C1E-8AC7-2158A03D1232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9A405-531F-4DB4-8E6A-FF2A53E0CCF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2470" yWindow="1100" windowWidth="19360" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$H$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$208</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -157,6 +157,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Robert Schwenn</author>
+    <author>sc</author>
   </authors>
   <commentList>
     <comment ref="A13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -297,6 +298,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="H13" authorId="1" shapeId="0" xr:uid="{BF5BADE9-1600-4792-AF5F-ADD4A82EB868}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">iTC = iTrassen-Codierung
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>iTC-Punktarten:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+-b   Bstg   Bahnsteig
+-f    PSx    Festpunkt
+-v   GVP   GVP
+-i    Gls     Gleis</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
@@ -332,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="523">
   <si>
     <t>GK.X</t>
   </si>
@@ -1813,12 +1854,206 @@
   <si>
     <t>Pkt.Kommentar</t>
   </si>
+  <si>
+    <t>iGeo-A0</t>
+  </si>
+  <si>
+    <t>PktNr</t>
+  </si>
+  <si>
+    <t>iTC: Vart FP/GVP</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>Km</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>HSOK</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>QG</t>
+  </si>
+  <si>
+    <t>HG</t>
+  </si>
+  <si>
+    <t>UebLi</t>
+  </si>
+  <si>
+    <t>UebRe</t>
+  </si>
+  <si>
+    <t>Feldname</t>
+  </si>
+  <si>
+    <t>iGeo-A0 =&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GeoTools Status</t>
+  </si>
+  <si>
+    <t>Ist</t>
+  </si>
+  <si>
+    <t>Soll</t>
+  </si>
+  <si>
+    <t>iTC: Überhöhung
+Ueb</t>
+  </si>
+  <si>
+    <t>Ist
+Soll</t>
+  </si>
+  <si>
+    <t>Heb</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>RaLGS</t>
+  </si>
+  <si>
+    <t>AbLGS</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>QGS</t>
+  </si>
+  <si>
+    <t>HGS</t>
+  </si>
+  <si>
+    <t>HDGM</t>
+  </si>
+  <si>
+    <t>ZDGM</t>
+  </si>
+  <si>
+    <t>Tm</t>
+  </si>
+  <si>
+    <t>QGT</t>
+  </si>
+  <si>
+    <t>HGT</t>
+  </si>
+  <si>
+    <t>QT</t>
+  </si>
+  <si>
+    <t>ZSOK</t>
+  </si>
+  <si>
+    <t>ZLGS</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>KmStatus</t>
+  </si>
+  <si>
+    <t>KmText</t>
+  </si>
+  <si>
+    <t>(Ist)</t>
+  </si>
+  <si>
+    <t>XA</t>
+  </si>
+  <si>
+    <t>YA</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>MiniR</t>
+  </si>
+  <si>
+    <t>MiniUeb</t>
+  </si>
+  <si>
+    <t>STB1</t>
+  </si>
+  <si>
+    <t>STB2</t>
+  </si>
+  <si>
+    <t>STB3</t>
+  </si>
+  <si>
+    <t>STB4</t>
+  </si>
+  <si>
+    <t>STB5</t>
+  </si>
+  <si>
+    <t>STB6</t>
+  </si>
+  <si>
+    <t>STB7</t>
+  </si>
+  <si>
+    <t>STB8</t>
+  </si>
+  <si>
+    <t>STB9</t>
+  </si>
+  <si>
+    <t>iTC: Punktart kurz</t>
+  </si>
+  <si>
+    <t>iTC: Punktart lang</t>
+  </si>
+  <si>
+    <t>iTC: VArt AbstBuch</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1912,8 +2147,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1935,6 +2185,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2174,7 +2436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -2292,12 +2554,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2336,6 +2592,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2452,7 +2726,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9766300" y="0"/>
+          <a:off x="9264650" y="0"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="731" y="0"/>
           <a:chExt cx="9765569" cy="450"/>
@@ -3367,6 +3641,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
@@ -3758,18 +4036,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -3923,7 +4201,7 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H208"/>
+  <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -3932,29 +4210,32 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.81640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="52.81640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" style="3" customWidth="1"/>
     <col min="6" max="6" width="27.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="49"/>
-    <col min="9" max="16384" width="11.1796875" style="1"/>
+    <col min="7" max="7" width="11.453125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="20.453125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="47"/>
+    <col min="11" max="16384" width="11.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:10" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="59"/>
       <c r="H1" s="44"/>
-    </row>
-    <row r="2" spans="1:8" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+    </row>
+    <row r="2" spans="1:10" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
       <c r="B2" s="28" t="s">
         <v>396</v>
@@ -3965,8 +4246,10 @@
       <c r="F2" s="28"/>
       <c r="G2" s="31"/>
       <c r="H2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
       <c r="B3" s="33" t="s">
         <v>141</v>
@@ -3977,8 +4260,10 @@
       <c r="F3" s="35"/>
       <c r="G3" s="37"/>
       <c r="H3" s="46"/>
-    </row>
-    <row r="4" spans="1:8" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+    </row>
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
         <v>397</v>
@@ -3989,8 +4274,10 @@
       <c r="F4" s="28"/>
       <c r="G4" s="31"/>
       <c r="H4" s="45"/>
-    </row>
-    <row r="5" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+    </row>
+    <row r="5" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32"/>
       <c r="B5" s="33" t="s">
         <v>170</v>
@@ -4001,8 +4288,10 @@
       <c r="F5" s="35"/>
       <c r="G5" s="37"/>
       <c r="H5" s="46"/>
-    </row>
-    <row r="6" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+    </row>
+    <row r="6" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
       <c r="B6" s="33" t="s">
         <v>156</v>
@@ -4013,8 +4302,10 @@
       <c r="F6" s="35"/>
       <c r="G6" s="37"/>
       <c r="H6" s="46"/>
-    </row>
-    <row r="7" spans="1:8" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="1:10" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27"/>
       <c r="B7" s="28" t="s">
         <v>139</v>
@@ -4025,8 +4316,10 @@
       <c r="F7" s="28"/>
       <c r="G7" s="31"/>
       <c r="H7" s="45"/>
-    </row>
-    <row r="8" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+    </row>
+    <row r="8" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="33" t="s">
         <v>398</v>
@@ -4037,8 +4330,10 @@
       <c r="F8" s="35"/>
       <c r="G8" s="37"/>
       <c r="H8" s="46"/>
-    </row>
-    <row r="9" spans="1:8" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+    </row>
+    <row r="9" spans="1:10" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
         <v>399</v>
@@ -4049,8 +4344,10 @@
       <c r="F9" s="28"/>
       <c r="G9" s="31"/>
       <c r="H9" s="45"/>
-    </row>
-    <row r="10" spans="1:8" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+    </row>
+    <row r="10" spans="1:10" s="17" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="28" t="s">
         <v>171</v>
@@ -4061,8 +4358,10 @@
       <c r="F10" s="28"/>
       <c r="G10" s="31"/>
       <c r="H10" s="45"/>
-    </row>
-    <row r="11" spans="1:8" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+    </row>
+    <row r="11" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="33" t="s">
         <v>172</v>
@@ -4073,8 +4372,10 @@
       <c r="F11" s="35"/>
       <c r="G11" s="37"/>
       <c r="H11" s="46"/>
-    </row>
-    <row r="12" spans="1:8" s="17" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+    </row>
+    <row r="12" spans="1:10" s="17" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="39"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -4083,8 +4384,10 @@
       <c r="F12" s="40"/>
       <c r="G12" s="42"/>
       <c r="H12" s="45"/>
-    </row>
-    <row r="13" spans="1:8" s="20" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+    </row>
+    <row r="13" spans="1:10" s="20" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>135</v>
       </c>
@@ -4100,13 +4403,21 @@
       <c r="E13" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:8" s="26" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="56"/>
+      <c r="H13" s="60" t="s">
+        <v>475</v>
+      </c>
+      <c r="I13" s="60" t="s">
+        <v>476</v>
+      </c>
+      <c r="J13" s="65">
+        <v>44257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="26" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>136</v>
       </c>
@@ -4120,11 +4431,17 @@
       <c r="G14" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="61" t="s">
+        <v>459</v>
+      </c>
+      <c r="I14" s="61" t="s">
+        <v>477</v>
+      </c>
+      <c r="J14" s="64" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="17" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" s="17" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>1</v>
       </c>
@@ -4143,8 +4460,10 @@
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="45"/>
-    </row>
-    <row r="16" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -4161,7 +4480,7 @@
       </c>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>3</v>
       </c>
@@ -4178,7 +4497,7 @@
       </c>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -4195,7 +4514,7 @@
       </c>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
         <v>5</v>
       </c>
@@ -4212,7 +4531,7 @@
       </c>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>6</v>
       </c>
@@ -4229,7 +4548,7 @@
       </c>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -4246,7 +4565,7 @@
       </c>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>8</v>
       </c>
@@ -4263,7 +4582,7 @@
       </c>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>9</v>
       </c>
@@ -4280,7 +4599,7 @@
       </c>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>10</v>
       </c>
@@ -4297,7 +4616,7 @@
       </c>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>11</v>
       </c>
@@ -4313,8 +4632,14 @@
         <v>61</v>
       </c>
       <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="47" t="s">
+        <v>460</v>
+      </c>
+      <c r="I25" s="47" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>12</v>
       </c>
@@ -4331,7 +4656,7 @@
       </c>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>13</v>
       </c>
@@ -4348,7 +4673,7 @@
       </c>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>14</v>
       </c>
@@ -4365,7 +4690,7 @@
       </c>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>15</v>
       </c>
@@ -4383,8 +4708,14 @@
         <v>61</v>
       </c>
       <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="47" t="s">
+        <v>462</v>
+      </c>
+      <c r="I29" s="47" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>16</v>
       </c>
@@ -4400,11 +4731,17 @@
         <v>61</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>17</v>
       </c>
@@ -4420,8 +4757,14 @@
         <v>61</v>
       </c>
       <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="48" t="s">
+        <v>520</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>18</v>
       </c>
@@ -4439,8 +4782,14 @@
         <v>61</v>
       </c>
       <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="48" t="s">
+        <v>521</v>
+      </c>
+      <c r="I32" s="47" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
         <v>19</v>
       </c>
@@ -4457,7 +4806,7 @@
       </c>
       <c r="G33" s="16"/>
     </row>
-    <row r="34" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>20</v>
       </c>
@@ -4474,7 +4823,7 @@
       </c>
       <c r="G34" s="16"/>
     </row>
-    <row r="35" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>21</v>
       </c>
@@ -4491,7 +4840,7 @@
       </c>
       <c r="G35" s="16"/>
     </row>
-    <row r="36" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>22</v>
       </c>
@@ -4508,7 +4857,7 @@
       </c>
       <c r="G36" s="16"/>
     </row>
-    <row r="37" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>23</v>
       </c>
@@ -4524,8 +4873,14 @@
         <v>61</v>
       </c>
       <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H37" s="47" t="s">
+        <v>461</v>
+      </c>
+      <c r="I37" s="47" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>24</v>
       </c>
@@ -4541,11 +4896,17 @@
         <v>61</v>
       </c>
       <c r="G38" s="16"/>
-      <c r="H38" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="48" t="s">
+        <v>522</v>
+      </c>
+      <c r="I38" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J38" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
         <v>25</v>
       </c>
@@ -4562,7 +4923,7 @@
       </c>
       <c r="G39" s="16"/>
     </row>
-    <row r="40" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>26</v>
       </c>
@@ -4579,7 +4940,7 @@
       </c>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>27</v>
       </c>
@@ -4596,7 +4957,7 @@
       </c>
       <c r="G41" s="16"/>
     </row>
-    <row r="42" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>28</v>
       </c>
@@ -4613,7 +4974,7 @@
       </c>
       <c r="G42" s="16"/>
     </row>
-    <row r="43" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>29</v>
       </c>
@@ -4630,7 +4991,7 @@
       </c>
       <c r="G43" s="16"/>
     </row>
-    <row r="44" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>30</v>
       </c>
@@ -4647,7 +5008,7 @@
       </c>
       <c r="G44" s="16"/>
     </row>
-    <row r="45" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
         <v>31</v>
       </c>
@@ -4664,7 +5025,7 @@
       </c>
       <c r="G45" s="16"/>
     </row>
-    <row r="46" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>32</v>
       </c>
@@ -4681,7 +5042,7 @@
       </c>
       <c r="G46" s="16"/>
     </row>
-    <row r="47" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>33</v>
       </c>
@@ -4698,7 +5059,7 @@
       </c>
       <c r="G47" s="16"/>
     </row>
-    <row r="48" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
         <v>34</v>
       </c>
@@ -5011,7 +5372,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>51</v>
       </c>
@@ -5030,7 +5391,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
         <v>52</v>
       </c>
@@ -5049,7 +5410,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>53</v>
       </c>
@@ -5068,7 +5429,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>54</v>
       </c>
@@ -5088,8 +5449,14 @@
       <c r="G68" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H68" s="47" t="s">
+        <v>463</v>
+      </c>
+      <c r="I68" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
         <v>55</v>
       </c>
@@ -5109,8 +5476,14 @@
       <c r="G69" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H69" s="47" t="s">
+        <v>464</v>
+      </c>
+      <c r="I69" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>56</v>
       </c>
@@ -5130,8 +5503,14 @@
       <c r="G70" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="47" t="s">
+        <v>465</v>
+      </c>
+      <c r="I70" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>57</v>
       </c>
@@ -5152,7 +5531,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="11">
         <v>58</v>
       </c>
@@ -5173,7 +5552,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>59</v>
       </c>
@@ -5194,7 +5573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>60</v>
       </c>
@@ -5215,7 +5594,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11">
         <v>61</v>
       </c>
@@ -5236,7 +5615,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>62</v>
       </c>
@@ -5257,7 +5636,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>63</v>
       </c>
@@ -5278,7 +5657,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11">
         <v>64</v>
       </c>
@@ -5299,7 +5678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>65</v>
       </c>
@@ -5320,7 +5699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>66</v>
       </c>
@@ -5341,7 +5720,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11">
         <v>67</v>
       </c>
@@ -5362,7 +5741,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>68</v>
       </c>
@@ -5383,7 +5762,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>69</v>
       </c>
@@ -5405,8 +5784,14 @@
       <c r="G83" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H83" s="47" t="s">
+        <v>466</v>
+      </c>
+      <c r="I83" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="11">
         <v>70</v>
       </c>
@@ -5428,8 +5813,14 @@
       <c r="G84" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H84" s="47" t="s">
+        <v>467</v>
+      </c>
+      <c r="I84" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>71</v>
       </c>
@@ -5447,8 +5838,14 @@
       <c r="G85" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H85" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="I85" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>72</v>
       </c>
@@ -5466,8 +5863,14 @@
       <c r="G86" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H86" s="47" t="s">
+        <v>504</v>
+      </c>
+      <c r="I86" s="63" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="11">
         <v>73</v>
       </c>
@@ -5486,7 +5889,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>74</v>
       </c>
@@ -5506,8 +5909,14 @@
       <c r="G88" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H88" s="47" t="s">
+        <v>468</v>
+      </c>
+      <c r="I88" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>75</v>
       </c>
@@ -5528,7 +5937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11">
         <v>76</v>
       </c>
@@ -5548,8 +5957,14 @@
       <c r="G90" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H90" s="47" t="s">
+        <v>469</v>
+      </c>
+      <c r="I90" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>77</v>
       </c>
@@ -5569,8 +5984,14 @@
       <c r="G91" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H91" s="47" t="s">
+        <v>470</v>
+      </c>
+      <c r="I91" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>78</v>
       </c>
@@ -5590,8 +6011,14 @@
       <c r="G92" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H92" s="47" t="s">
+        <v>471</v>
+      </c>
+      <c r="I92" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="11">
         <v>79</v>
       </c>
@@ -5611,8 +6038,14 @@
       <c r="G93" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H93" s="47" t="s">
+        <v>472</v>
+      </c>
+      <c r="I93" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>80</v>
       </c>
@@ -5632,8 +6065,14 @@
       <c r="G94" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H94" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="I94" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>81</v>
       </c>
@@ -5653,8 +6092,14 @@
       <c r="G95" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H95" s="47" t="s">
+        <v>502</v>
+      </c>
+      <c r="I95" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="11">
         <v>82</v>
       </c>
@@ -5674,11 +6119,17 @@
       <c r="G96" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H96" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H96" s="47" t="s">
+        <v>495</v>
+      </c>
+      <c r="I96" s="47" t="s">
+        <v>478</v>
+      </c>
+      <c r="J96" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>83</v>
       </c>
@@ -5698,11 +6149,17 @@
       <c r="G97" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H97" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H97" s="47" t="s">
+        <v>498</v>
+      </c>
+      <c r="I97" s="47" t="s">
+        <v>478</v>
+      </c>
+      <c r="J97" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>84</v>
       </c>
@@ -5722,8 +6179,14 @@
       <c r="G98" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H98" s="47" t="s">
+        <v>496</v>
+      </c>
+      <c r="I98" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="11">
         <v>85</v>
       </c>
@@ -5743,8 +6206,14 @@
       <c r="G99" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H99" s="47" t="s">
+        <v>497</v>
+      </c>
+      <c r="I99" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>86</v>
       </c>
@@ -5764,8 +6233,14 @@
       <c r="G100" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H100" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="I100" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>87</v>
       </c>
@@ -5785,8 +6260,14 @@
       <c r="G101" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H101" s="47" t="s">
+        <v>490</v>
+      </c>
+      <c r="I101" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="11">
         <v>88</v>
       </c>
@@ -5806,8 +6287,14 @@
       <c r="G102" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H102" s="47" t="s">
+        <v>491</v>
+      </c>
+      <c r="I102" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>89</v>
       </c>
@@ -5827,8 +6314,14 @@
       <c r="G103" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H103" s="47" t="s">
+        <v>492</v>
+      </c>
+      <c r="I103" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>90</v>
       </c>
@@ -5848,8 +6341,14 @@
       <c r="G104" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H104" s="47" t="s">
+        <v>488</v>
+      </c>
+      <c r="I104" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="11">
         <v>91</v>
       </c>
@@ -5868,7 +6367,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>92</v>
       </c>
@@ -5887,7 +6386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>93</v>
       </c>
@@ -5906,7 +6405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="11">
         <v>94</v>
       </c>
@@ -5925,7 +6424,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>95</v>
       </c>
@@ -5944,7 +6443,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>96</v>
       </c>
@@ -5963,7 +6462,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="11">
         <v>97</v>
       </c>
@@ -5982,7 +6481,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>98</v>
       </c>
@@ -6001,7 +6500,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>99</v>
       </c>
@@ -6021,8 +6520,14 @@
       <c r="G113" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H113" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="I113" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="11">
         <v>100</v>
       </c>
@@ -6042,8 +6547,14 @@
       <c r="G114" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H114" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="I114" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>101</v>
       </c>
@@ -6063,8 +6574,15 @@
       <c r="G115" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H115" s="62" t="s">
+        <v>480</v>
+      </c>
+      <c r="I115" s="62" t="s">
+        <v>481</v>
+      </c>
+      <c r="J115" s="62"/>
+    </row>
+    <row r="116" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>102</v>
       </c>
@@ -6085,7 +6603,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="11">
         <v>103</v>
       </c>
@@ -6105,11 +6623,17 @@
       <c r="G117" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H117" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H117" s="47" t="s">
+        <v>473</v>
+      </c>
+      <c r="I117" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J117" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>104</v>
       </c>
@@ -6129,11 +6653,17 @@
       <c r="G118" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H118" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H118" s="47" t="s">
+        <v>474</v>
+      </c>
+      <c r="I118" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J118" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>105</v>
       </c>
@@ -6153,8 +6683,14 @@
       <c r="G119" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H119" s="47" t="s">
+        <v>499</v>
+      </c>
+      <c r="I119" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="11">
         <v>106</v>
       </c>
@@ -6174,11 +6710,17 @@
       <c r="G120" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H120" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H120" s="47" t="s">
+        <v>500</v>
+      </c>
+      <c r="I120" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J120" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>107</v>
       </c>
@@ -6198,8 +6740,14 @@
       <c r="G121" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H121" s="47" t="s">
+        <v>482</v>
+      </c>
+      <c r="I121" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>108</v>
       </c>
@@ -6219,8 +6767,14 @@
       <c r="G122" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H122" s="47" t="s">
+        <v>483</v>
+      </c>
+      <c r="I122" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="11">
         <v>109</v>
       </c>
@@ -6240,8 +6794,14 @@
       <c r="G123" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H123" s="47" t="s">
+        <v>484</v>
+      </c>
+      <c r="I123" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>110</v>
       </c>
@@ -6261,8 +6821,14 @@
       <c r="G124" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H124" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="I124" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>111</v>
       </c>
@@ -6281,7 +6847,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="11">
         <v>112</v>
       </c>
@@ -6302,7 +6868,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>113</v>
       </c>
@@ -6322,11 +6888,17 @@
       <c r="G127" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H127" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H127" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="I127" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J127" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>114</v>
       </c>
@@ -6346,11 +6918,17 @@
       <c r="G128" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H128" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H128" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="I128" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J128" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="11">
         <v>115</v>
       </c>
@@ -6370,11 +6948,17 @@
       <c r="G129" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H129" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H129" s="47" t="s">
+        <v>508</v>
+      </c>
+      <c r="I129" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J129" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>116</v>
       </c>
@@ -6394,11 +6978,17 @@
       <c r="G130" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H130" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H130" s="47" t="s">
+        <v>509</v>
+      </c>
+      <c r="I130" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J130" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>117</v>
       </c>
@@ -6418,11 +7008,17 @@
       <c r="G131" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H131" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H131" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="I131" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="J131" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="11">
         <v>118</v>
       </c>
@@ -6440,11 +7036,17 @@
       <c r="G132" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H132" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H132" s="47" t="s">
+        <v>511</v>
+      </c>
+      <c r="I132" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J132" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>119</v>
       </c>
@@ -6462,11 +7064,17 @@
       <c r="G133" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H133" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H133" s="47" t="s">
+        <v>512</v>
+      </c>
+      <c r="I133" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J133" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>120</v>
       </c>
@@ -6484,11 +7092,17 @@
       <c r="G134" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H134" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H134" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="I134" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J134" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="11">
         <v>121</v>
       </c>
@@ -6506,11 +7120,17 @@
       <c r="G135" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H135" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H135" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="I135" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J135" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>122</v>
       </c>
@@ -6528,11 +7148,17 @@
       <c r="G136" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H136" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H136" s="47" t="s">
+        <v>515</v>
+      </c>
+      <c r="I136" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J136" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>123</v>
       </c>
@@ -6550,11 +7176,17 @@
       <c r="G137" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H137" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H137" s="47" t="s">
+        <v>516</v>
+      </c>
+      <c r="I137" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J137" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="11">
         <v>124</v>
       </c>
@@ -6572,11 +7204,17 @@
       <c r="G138" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H138" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H138" s="47" t="s">
+        <v>517</v>
+      </c>
+      <c r="I138" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J138" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>125</v>
       </c>
@@ -6594,11 +7232,17 @@
       <c r="G139" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H139" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H139" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="I139" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J139" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>126</v>
       </c>
@@ -6616,11 +7260,17 @@
       <c r="G140" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H140" s="49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H140" s="47" t="s">
+        <v>519</v>
+      </c>
+      <c r="I140" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="J140" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="11">
         <v>127</v>
       </c>
@@ -6640,8 +7290,14 @@
       <c r="G141" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H141" s="47" t="s">
+        <v>493</v>
+      </c>
+      <c r="I141" s="47" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>128</v>
       </c>
@@ -6661,8 +7317,14 @@
       <c r="G142" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H142" s="47" t="s">
+        <v>494</v>
+      </c>
+      <c r="I142" s="47" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>129</v>
       </c>
@@ -6681,7 +7343,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="11">
         <v>130</v>
       </c>
@@ -7933,7 +8595,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A14:H208" xr:uid="{168694DD-CE74-4BD8-9923-46F7E34A5FB5}"/>
+  <autoFilter ref="A14:J208" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>

<commit_message>
Zerlegen der iTrassen-Codierung: Anpassung an Rstyx.Utilities, Teil 1
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9A405-531F-4DB4-8E6A-FF2A53E0CCF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B66D25-16EA-43D7-8907-CB126EB2EEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$211</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="529">
   <si>
     <t>GK.X</t>
   </si>
@@ -2047,6 +2047,24 @@
   </si>
   <si>
     <t>iTC: VArt AbstBuch</t>
+  </si>
+  <si>
+    <t>Messung Bildname ist gültig (als Dateiname)</t>
+  </si>
+  <si>
+    <t>Mess.BildName.existiert</t>
+  </si>
+  <si>
+    <t>Messung Bilddatei exitiert</t>
+  </si>
+  <si>
+    <t>Mess.BildName.Winlue</t>
+  </si>
+  <si>
+    <t>Messung Bildname ist Winlue-kompatibel</t>
+  </si>
+  <si>
+    <t>Mess.BildName.gueltig</t>
   </si>
 </sst>
 </file>
@@ -2560,6 +2578,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2592,24 +2628,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2726,10 +2744,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9264650" y="0"/>
+          <a:off x="9474200" y="0"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="731" y="0"/>
-          <a:chExt cx="9765569" cy="450"/>
+          <a:chExt cx="9473469" cy="450"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -2791,7 +2809,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="9766300" y="0"/>
+                <a:off x="9474200" y="0"/>
                 <a:ext cx="0" cy="0"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -3641,10 +3659,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
@@ -4036,18 +4050,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -4201,16 +4215,16 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" style="2" customWidth="1"/>
     <col min="3" max="3" width="52.81640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.6328125" style="3" customWidth="1"/>
@@ -4222,15 +4236,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -4403,17 +4417,17 @@
       <c r="E13" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="60" t="s">
+      <c r="G13" s="62"/>
+      <c r="H13" s="49" t="s">
         <v>475</v>
       </c>
-      <c r="I13" s="60" t="s">
+      <c r="I13" s="49" t="s">
         <v>476</v>
       </c>
-      <c r="J13" s="65">
+      <c r="J13" s="54">
         <v>44257</v>
       </c>
     </row>
@@ -4431,13 +4445,13 @@
       <c r="G14" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="61" t="s">
+      <c r="H14" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="I14" s="61" t="s">
+      <c r="I14" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="J14" s="53" t="s">
         <v>454</v>
       </c>
     </row>
@@ -5841,7 +5855,7 @@
       <c r="H85" s="47" t="s">
         <v>503</v>
       </c>
-      <c r="I85" s="63" t="s">
+      <c r="I85" s="52" t="s">
         <v>505</v>
       </c>
     </row>
@@ -5866,7 +5880,7 @@
       <c r="H86" s="47" t="s">
         <v>504</v>
       </c>
-      <c r="I86" s="63" t="s">
+      <c r="I86" s="52" t="s">
         <v>505</v>
       </c>
     </row>
@@ -6574,13 +6588,13 @@
       <c r="G115" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H115" s="62" t="s">
+      <c r="H115" s="51" t="s">
         <v>480</v>
       </c>
-      <c r="I115" s="62" t="s">
+      <c r="I115" s="51" t="s">
         <v>481</v>
       </c>
-      <c r="J115" s="62"/>
+      <c r="J115" s="51"/>
     </row>
     <row r="116" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
@@ -8131,14 +8145,14 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="1">
+      <c r="A185" s="11">
         <v>171</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>343</v>
+        <v>528</v>
       </c>
       <c r="C185" s="15" t="s">
-        <v>340</v>
+        <v>523</v>
       </c>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
@@ -8150,14 +8164,14 @@
       </c>
     </row>
     <row r="186" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="11">
+      <c r="A186" s="1">
         <v>172</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>349</v>
+        <v>524</v>
       </c>
       <c r="C186" s="15" t="s">
-        <v>345</v>
+        <v>525</v>
       </c>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
@@ -8173,10 +8187,10 @@
         <v>173</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>350</v>
+        <v>526</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>346</v>
+        <v>527</v>
       </c>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
@@ -8188,14 +8202,14 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="1">
+      <c r="A188" s="11">
         <v>174</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15"/>
@@ -8207,14 +8221,14 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="11">
+      <c r="A189" s="1">
         <v>175</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C189" s="15" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15"/>
@@ -8226,19 +8240,19 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="1">
+      <c r="A190" s="11">
         <v>176</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15"/>
       <c r="F190" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G190" s="16" t="s">
         <v>57</v>
@@ -8249,52 +8263,50 @@
         <v>177</v>
       </c>
       <c r="B191" s="14" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C191" s="15" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
       <c r="F191" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G191" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="11">
+      <c r="A192" s="1">
         <v>178</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C192" s="15" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
       <c r="F192" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="G192" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="1">
+      <c r="A193" s="11">
         <v>179</v>
       </c>
       <c r="B193" s="14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C193" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="D193" s="15" t="s">
-        <v>44</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="D193" s="15"/>
       <c r="E193" s="15"/>
       <c r="F193" s="15" t="s">
         <v>337</v>
@@ -8308,14 +8320,12 @@
         <v>180</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="D194" s="15" t="s">
-        <v>44</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="15" t="s">
         <v>337</v>
@@ -8329,14 +8339,12 @@
         <v>181</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="D195" s="15" t="s">
-        <v>44</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="D195" s="15"/>
       <c r="E195" s="15"/>
       <c r="F195" s="15" t="s">
         <v>337</v>
@@ -8350,10 +8358,10 @@
         <v>182</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D196" s="15" t="s">
         <v>44</v>
@@ -8371,12 +8379,14 @@
         <v>183</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="D197" s="15"/>
+        <v>361</v>
+      </c>
+      <c r="D197" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="E197" s="15"/>
       <c r="F197" s="15" t="s">
         <v>337</v>
@@ -8390,12 +8400,14 @@
         <v>184</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="D198" s="15"/>
+        <v>362</v>
+      </c>
+      <c r="D198" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="E198" s="15"/>
       <c r="F198" s="15" t="s">
         <v>337</v>
@@ -8409,12 +8421,14 @@
         <v>185</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
       <c r="C199" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="D199" s="15"/>
+        <v>363</v>
+      </c>
+      <c r="D199" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="E199" s="15"/>
       <c r="F199" s="15" t="s">
         <v>337</v>
@@ -8424,14 +8438,14 @@
       </c>
     </row>
     <row r="200" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="1">
+      <c r="A200" s="11">
         <v>186</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C200" s="15" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
@@ -8443,14 +8457,14 @@
       </c>
     </row>
     <row r="201" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="11">
+      <c r="A201" s="1">
         <v>187</v>
       </c>
       <c r="B201" s="14" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C201" s="15" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
@@ -8466,10 +8480,10 @@
         <v>188</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="C202" s="15" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
@@ -8481,14 +8495,14 @@
       </c>
     </row>
     <row r="203" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="1">
+      <c r="A203" s="11">
         <v>189</v>
       </c>
       <c r="B203" s="14" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="C203" s="15" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="D203" s="15"/>
       <c r="E203" s="15"/>
@@ -8500,14 +8514,14 @@
       </c>
     </row>
     <row r="204" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="11">
+      <c r="A204" s="1">
         <v>190</v>
       </c>
       <c r="B204" s="14" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="C204" s="15" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="D204" s="15"/>
       <c r="E204" s="15"/>
@@ -8519,14 +8533,14 @@
       </c>
     </row>
     <row r="205" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="1">
+      <c r="A205" s="11">
         <v>191</v>
       </c>
       <c r="B205" s="14" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C205" s="15" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D205" s="15"/>
       <c r="E205" s="15"/>
@@ -8542,10 +8556,10 @@
         <v>192</v>
       </c>
       <c r="B206" s="14" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="C206" s="15" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="D206" s="15"/>
       <c r="E206" s="15"/>
@@ -8557,14 +8571,14 @@
       </c>
     </row>
     <row r="207" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A207" s="11">
+      <c r="A207" s="1">
         <v>193</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="C207" s="15" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D207" s="15"/>
       <c r="E207" s="15"/>
@@ -8576,14 +8590,14 @@
       </c>
     </row>
     <row r="208" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="1">
+      <c r="A208" s="11">
         <v>194</v>
       </c>
       <c r="B208" s="14" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="C208" s="15" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D208" s="15"/>
       <c r="E208" s="15"/>
@@ -8594,8 +8608,65 @@
         <v>57</v>
       </c>
     </row>
+    <row r="209" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="1">
+        <v>195</v>
+      </c>
+      <c r="B209" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="C209" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="D209" s="15"/>
+      <c r="E209" s="15"/>
+      <c r="F209" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="G209" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A210" s="11">
+        <v>196</v>
+      </c>
+      <c r="B210" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="C210" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="D210" s="15"/>
+      <c r="E210" s="15"/>
+      <c r="F210" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="G210" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A211" s="1">
+        <v>197</v>
+      </c>
+      <c r="B211" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="C211" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="D211" s="15"/>
+      <c r="E211" s="15"/>
+      <c r="F211" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="G211" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A14:J208" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
+  <autoFilter ref="A14:J211" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>

<commit_message>
CimpTrassenkoo und Konfig: Neues Feld "Tra.NameAcfg" für iGeo-TK
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{064461DE-83D3-42B9-882F-27470F602570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7BB1770-AABD-4210-851A-DA3146DAE92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="980" windowWidth="19540" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3190" yWindow="1820" windowWidth="19540" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$211</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$212</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="529">
   <si>
     <t>GK.X</t>
   </si>
@@ -2040,6 +2040,12 @@
   </si>
   <si>
     <t>Mess.BildName.gueltig</t>
+  </si>
+  <si>
+    <t>Tra.NameAcfg</t>
+  </si>
+  <si>
+    <t>Name Trassenkonfiguration</t>
   </si>
 </sst>
 </file>
@@ -4178,10 +4184,10 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J211"/>
+  <dimension ref="A1:J212"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105:E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -6327,10 +6333,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>14</v>
+        <v>527</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>40</v>
+        <v>528</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -6346,10 +6352,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D106" s="14"/>
       <c r="E106" s="14"/>
@@ -6365,13 +6371,15 @@
         <v>93</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
+      <c r="E107" s="14" t="s">
+        <v>527</v>
+      </c>
       <c r="F107" s="14" t="s">
         <v>25</v>
       </c>
@@ -6384,10 +6392,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -6403,10 +6411,10 @@
         <v>95</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>262</v>
+        <v>42</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -6422,10 +6430,10 @@
         <v>96</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
@@ -6441,10 +6449,10 @@
         <v>97</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>259</v>
+        <v>160</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
@@ -6460,10 +6468,10 @@
         <v>98</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
@@ -6479,14 +6487,12 @@
         <v>99</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>18</v>
+        <v>260</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="D113" s="14"/>
       <c r="E113" s="14"/>
       <c r="F113" s="14" t="s">
         <v>25</v>
@@ -6494,25 +6500,19 @@
       <c r="G113" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H113" s="46" t="s">
-        <v>484</v>
-      </c>
-      <c r="I113" s="46" t="s">
-        <v>477</v>
-      </c>
     </row>
     <row r="114" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10">
         <v>100</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E114" s="14"/>
       <c r="F114" s="14" t="s">
@@ -6522,21 +6522,21 @@
         <v>57</v>
       </c>
       <c r="H114" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I114" s="46" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>101</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>330</v>
+        <v>28</v>
       </c>
       <c r="D115" s="14" t="s">
         <v>44</v>
@@ -6548,23 +6548,22 @@
       <c r="G115" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H115" s="50" t="s">
-        <v>478</v>
-      </c>
-      <c r="I115" s="50" t="s">
-        <v>479</v>
-      </c>
-      <c r="J115" s="50"/>
-    </row>
-    <row r="116" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H115" s="46" t="s">
+        <v>485</v>
+      </c>
+      <c r="I115" s="46" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>102</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>332</v>
+        <v>20</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>44</v>
@@ -6576,16 +6575,23 @@
       <c r="G116" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="H116" s="50" t="s">
+        <v>478</v>
+      </c>
+      <c r="I116" s="50" t="s">
+        <v>479</v>
+      </c>
+      <c r="J116" s="50"/>
     </row>
     <row r="117" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10">
         <v>103</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>430</v>
+        <v>332</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>431</v>
+        <v>331</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>44</v>
@@ -6597,25 +6603,16 @@
       <c r="G117" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H117" s="46" t="s">
-        <v>471</v>
-      </c>
-      <c r="I117" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J117" s="46" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="118" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>104</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>44</v>
@@ -6628,7 +6625,7 @@
         <v>57</v>
       </c>
       <c r="H118" s="46" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I118" s="46" t="s">
         <v>477</v>
@@ -6642,10 +6639,10 @@
         <v>105</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="D119" s="14" t="s">
         <v>44</v>
@@ -6658,10 +6655,13 @@
         <v>57</v>
       </c>
       <c r="H119" s="46" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
       <c r="I119" s="46" t="s">
         <v>477</v>
+      </c>
+      <c r="J119" s="46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6669,10 +6669,10 @@
         <v>106</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>420</v>
+        <v>19</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D120" s="14" t="s">
         <v>44</v>
@@ -6685,13 +6685,10 @@
         <v>57</v>
       </c>
       <c r="H120" s="46" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I120" s="46" t="s">
         <v>477</v>
-      </c>
-      <c r="J120" s="46" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6699,10 +6696,10 @@
         <v>107</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>38</v>
+        <v>420</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>27</v>
+        <v>421</v>
       </c>
       <c r="D121" s="14" t="s">
         <v>44</v>
@@ -6715,10 +6712,13 @@
         <v>57</v>
       </c>
       <c r="H121" s="46" t="s">
-        <v>480</v>
+        <v>498</v>
       </c>
       <c r="I121" s="46" t="s">
         <v>477</v>
+      </c>
+      <c r="J121" s="46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6726,13 +6726,13 @@
         <v>108</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>408</v>
+        <v>38</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>409</v>
+        <v>27</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E122" s="14"/>
       <c r="F122" s="14" t="s">
@@ -6742,7 +6742,7 @@
         <v>57</v>
       </c>
       <c r="H122" s="46" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I122" s="46" t="s">
         <v>477</v>
@@ -6753,13 +6753,13 @@
         <v>109</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>385</v>
+        <v>409</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E123" s="14"/>
       <c r="F123" s="14" t="s">
@@ -6769,7 +6769,7 @@
         <v>57</v>
       </c>
       <c r="H123" s="46" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I123" s="46" t="s">
         <v>477</v>
@@ -6780,10 +6780,10 @@
         <v>110</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D124" s="14" t="s">
         <v>44</v>
@@ -6796,7 +6796,7 @@
         <v>57</v>
       </c>
       <c r="H124" s="46" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I124" s="46" t="s">
         <v>477</v>
@@ -6807,12 +6807,14 @@
         <v>111</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="D125" s="14"/>
+        <v>384</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E125" s="14"/>
       <c r="F125" s="14" t="s">
         <v>25</v>
@@ -6820,20 +6822,24 @@
       <c r="G125" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="H125" s="46" t="s">
+        <v>483</v>
+      </c>
+      <c r="I125" s="46" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="126" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="10">
         <v>112</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="D126" s="14"/>
       <c r="E126" s="14"/>
       <c r="F126" s="14" t="s">
         <v>25</v>
@@ -6847,10 +6853,10 @@
         <v>113</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="D127" s="14" t="s">
         <v>44</v>
@@ -6862,25 +6868,16 @@
       <c r="G127" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H127" s="46" t="s">
-        <v>504</v>
-      </c>
-      <c r="I127" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J127" s="46" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="128" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>114</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D128" s="14" t="s">
         <v>44</v>
@@ -6893,7 +6890,7 @@
         <v>57</v>
       </c>
       <c r="H128" s="46" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I128" s="46" t="s">
         <v>477</v>
@@ -6907,10 +6904,10 @@
         <v>115</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>44</v>
@@ -6923,7 +6920,7 @@
         <v>57</v>
       </c>
       <c r="H129" s="46" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I129" s="46" t="s">
         <v>477</v>
@@ -6937,10 +6934,10 @@
         <v>116</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>44</v>
@@ -6953,7 +6950,7 @@
         <v>57</v>
       </c>
       <c r="H130" s="46" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I130" s="46" t="s">
         <v>477</v>
@@ -6967,10 +6964,10 @@
         <v>117</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>44</v>
@@ -6983,7 +6980,7 @@
         <v>57</v>
       </c>
       <c r="H131" s="46" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I131" s="46" t="s">
         <v>477</v>
@@ -6997,12 +6994,14 @@
         <v>118</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="D132" s="14"/>
+        <v>418</v>
+      </c>
+      <c r="D132" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E132" s="14"/>
       <c r="F132" s="14" t="s">
         <v>25</v>
@@ -7011,10 +7010,10 @@
         <v>57</v>
       </c>
       <c r="H132" s="46" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I132" s="46" t="s">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="J132" s="46" t="s">
         <v>57</v>
@@ -7025,10 +7024,10 @@
         <v>119</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="D133" s="14"/>
       <c r="E133" s="14"/>
@@ -7039,7 +7038,7 @@
         <v>57</v>
       </c>
       <c r="H133" s="46" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I133" s="46" t="s">
         <v>503</v>
@@ -7053,10 +7052,10 @@
         <v>120</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
@@ -7067,7 +7066,7 @@
         <v>57</v>
       </c>
       <c r="H134" s="46" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I134" s="46" t="s">
         <v>503</v>
@@ -7081,10 +7080,10 @@
         <v>121</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
@@ -7095,7 +7094,7 @@
         <v>57</v>
       </c>
       <c r="H135" s="46" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I135" s="46" t="s">
         <v>503</v>
@@ -7109,10 +7108,10 @@
         <v>122</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
@@ -7123,7 +7122,7 @@
         <v>57</v>
       </c>
       <c r="H136" s="46" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I136" s="46" t="s">
         <v>503</v>
@@ -7137,10 +7136,10 @@
         <v>123</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
@@ -7151,7 +7150,7 @@
         <v>57</v>
       </c>
       <c r="H137" s="46" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I137" s="46" t="s">
         <v>503</v>
@@ -7165,10 +7164,10 @@
         <v>124</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
@@ -7179,7 +7178,7 @@
         <v>57</v>
       </c>
       <c r="H138" s="46" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I138" s="46" t="s">
         <v>503</v>
@@ -7193,10 +7192,10 @@
         <v>125</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
@@ -7207,7 +7206,7 @@
         <v>57</v>
       </c>
       <c r="H139" s="46" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I139" s="46" t="s">
         <v>503</v>
@@ -7221,10 +7220,10 @@
         <v>126</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
@@ -7235,7 +7234,7 @@
         <v>57</v>
       </c>
       <c r="H140" s="46" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I140" s="46" t="s">
         <v>503</v>
@@ -7249,26 +7248,27 @@
         <v>127</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>250</v>
+        <v>443</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="D141" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="D141" s="14"/>
       <c r="E141" s="14"/>
       <c r="F141" s="14" t="s">
-        <v>254</v>
+        <v>25</v>
       </c>
       <c r="G141" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H141" s="46" t="s">
-        <v>491</v>
+        <v>517</v>
       </c>
       <c r="I141" s="46" t="s">
-        <v>476</v>
+        <v>503</v>
+      </c>
+      <c r="J141" s="46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="142" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7276,10 +7276,10 @@
         <v>128</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D142" s="14" t="s">
         <v>44</v>
@@ -7292,10 +7292,10 @@
         <v>57</v>
       </c>
       <c r="H142" s="46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I142" s="46" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="143" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7303,12 +7303,14 @@
         <v>129</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D143" s="14"/>
+        <v>253</v>
+      </c>
+      <c r="D143" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E143" s="14"/>
       <c r="F143" s="14" t="s">
         <v>254</v>
@@ -7316,21 +7318,27 @@
       <c r="G143" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="H143" s="46" t="s">
+        <v>492</v>
+      </c>
+      <c r="I143" s="46" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="144" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="10">
         <v>130</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="D144" s="14"/>
       <c r="E144" s="14"/>
       <c r="F144" s="14" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="G144" s="15" t="s">
         <v>57</v>
@@ -7341,10 +7349,10 @@
         <v>131</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
@@ -7360,10 +7368,10 @@
         <v>132</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
@@ -7379,10 +7387,10 @@
         <v>133</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
@@ -7398,10 +7406,10 @@
         <v>134</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
@@ -7417,10 +7425,10 @@
         <v>135</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
@@ -7436,10 +7444,10 @@
         <v>136</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
@@ -7455,14 +7463,12 @@
         <v>137</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D151" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D151" s="14"/>
       <c r="E151" s="14"/>
       <c r="F151" s="14" t="s">
         <v>218</v>
@@ -7476,12 +7482,14 @@
         <v>138</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="D152" s="14"/>
+        <v>215</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="E152" s="14"/>
       <c r="F152" s="14" t="s">
         <v>218</v>
@@ -7495,10 +7503,10 @@
         <v>139</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="D153" s="14"/>
       <c r="E153" s="14"/>
@@ -7514,10 +7522,10 @@
         <v>140</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
@@ -7533,10 +7541,10 @@
         <v>141</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
@@ -7552,10 +7560,10 @@
         <v>142</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
@@ -7571,10 +7579,10 @@
         <v>143</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
@@ -7590,10 +7598,10 @@
         <v>144</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
@@ -7609,10 +7617,10 @@
         <v>145</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
@@ -7628,10 +7636,10 @@
         <v>146</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
@@ -7647,14 +7655,12 @@
         <v>147</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D161" s="14"/>
       <c r="E161" s="14"/>
       <c r="F161" s="14" t="s">
         <v>218</v>
@@ -7668,12 +7674,14 @@
         <v>148</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D162" s="14"/>
+        <v>233</v>
+      </c>
+      <c r="D162" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E162" s="14"/>
       <c r="F162" s="14" t="s">
         <v>218</v>
@@ -7687,10 +7695,10 @@
         <v>149</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D163" s="14"/>
       <c r="E163" s="14"/>
@@ -7706,10 +7714,10 @@
         <v>150</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
@@ -7725,10 +7733,10 @@
         <v>151</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
@@ -7744,10 +7752,10 @@
         <v>152</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
@@ -7763,10 +7771,10 @@
         <v>153</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
@@ -7782,15 +7790,15 @@
         <v>154</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
       <c r="F168" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G168" s="15" t="s">
         <v>57</v>
@@ -7801,14 +7809,12 @@
         <v>155</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D169" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D169" s="14"/>
       <c r="E169" s="14"/>
       <c r="F169" s="14" t="s">
         <v>217</v>
@@ -7822,12 +7828,14 @@
         <v>156</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D170" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="D170" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E170" s="14"/>
       <c r="F170" s="14" t="s">
         <v>217</v>
@@ -7841,10 +7849,10 @@
         <v>157</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D171" s="14"/>
       <c r="E171" s="14"/>
@@ -7860,14 +7868,12 @@
         <v>158</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>301</v>
+        <v>186</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="D172" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="D172" s="14"/>
       <c r="E172" s="14"/>
       <c r="F172" s="14" t="s">
         <v>217</v>
@@ -7881,15 +7887,17 @@
         <v>159</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="D173" s="14"/>
+        <v>302</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E173" s="14"/>
       <c r="F173" s="14" t="s">
-        <v>313</v>
+        <v>217</v>
       </c>
       <c r="G173" s="15" t="s">
         <v>57</v>
@@ -7900,10 +7908,10 @@
         <v>160</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D174" s="14"/>
       <c r="E174" s="14"/>
@@ -7919,10 +7927,10 @@
         <v>161</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
@@ -7938,10 +7946,10 @@
         <v>162</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
@@ -7957,10 +7965,10 @@
         <v>163</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
@@ -7976,10 +7984,10 @@
         <v>164</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
@@ -7995,10 +8003,10 @@
         <v>165</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
@@ -8014,10 +8022,10 @@
         <v>166</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
@@ -8033,15 +8041,15 @@
         <v>167</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
       <c r="F181" s="14" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="G181" s="15" t="s">
         <v>57</v>
@@ -8052,10 +8060,10 @@
         <v>168</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>377</v>
+        <v>342</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>378</v>
+        <v>339</v>
       </c>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
@@ -8071,10 +8079,10 @@
         <v>169</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
@@ -8090,10 +8098,10 @@
         <v>170</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
@@ -8105,14 +8113,14 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="10">
+      <c r="A185">
         <v>171</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>526</v>
+        <v>340</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>521</v>
+        <v>337</v>
       </c>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
@@ -8124,14 +8132,14 @@
       </c>
     </row>
     <row r="186" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186">
+      <c r="A186" s="10">
         <v>172</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
@@ -8147,10 +8155,10 @@
         <v>173</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C187" s="14" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
@@ -8162,14 +8170,14 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="10">
+      <c r="A188">
         <v>174</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>341</v>
+        <v>524</v>
       </c>
       <c r="C188" s="14" t="s">
-        <v>338</v>
+        <v>525</v>
       </c>
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
@@ -8181,14 +8189,14 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189">
+      <c r="A189" s="10">
         <v>175</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
@@ -8200,14 +8208,14 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="10">
+      <c r="A190">
         <v>176</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C190" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
@@ -8223,10 +8231,10 @@
         <v>177</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
@@ -8238,14 +8246,14 @@
       </c>
     </row>
     <row r="192" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192">
+      <c r="A192" s="10">
         <v>178</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
@@ -8257,19 +8265,19 @@
       </c>
     </row>
     <row r="193" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="10">
+      <c r="A193">
         <v>179</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="14" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G193" s="15" t="s">
         <v>57</v>
@@ -8280,10 +8288,10 @@
         <v>180</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
@@ -8299,10 +8307,10 @@
         <v>181</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
@@ -8318,14 +8326,12 @@
         <v>182</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="D196" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="D196" s="14"/>
       <c r="E196" s="14"/>
       <c r="F196" s="14" t="s">
         <v>335</v>
@@ -8339,10 +8345,10 @@
         <v>183</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D197" s="14" t="s">
         <v>44</v>
@@ -8360,10 +8366,10 @@
         <v>184</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D198" s="14" t="s">
         <v>44</v>
@@ -8381,10 +8387,10 @@
         <v>185</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D199" s="14" t="s">
         <v>44</v>
@@ -8398,16 +8404,18 @@
       </c>
     </row>
     <row r="200" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="10">
+      <c r="A200">
         <v>186</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="D200" s="14"/>
+        <v>361</v>
+      </c>
+      <c r="D200" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E200" s="14"/>
       <c r="F200" s="14" t="s">
         <v>335</v>
@@ -8417,14 +8425,14 @@
       </c>
     </row>
     <row r="201" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201">
+      <c r="A201" s="10">
         <v>187</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D201" s="14"/>
       <c r="E201" s="14"/>
@@ -8440,10 +8448,10 @@
         <v>188</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
@@ -8455,14 +8463,14 @@
       </c>
     </row>
     <row r="203" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="10">
+      <c r="A203">
         <v>189</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>373</v>
+        <v>400</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
@@ -8474,14 +8482,14 @@
       </c>
     </row>
     <row r="204" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204">
+      <c r="A204" s="10">
         <v>190</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
@@ -8493,14 +8501,14 @@
       </c>
     </row>
     <row r="205" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="10">
+      <c r="A205">
         <v>191</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
@@ -8516,10 +8524,10 @@
         <v>192</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
@@ -8531,14 +8539,14 @@
       </c>
     </row>
     <row r="207" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A207">
+      <c r="A207" s="10">
         <v>193</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
@@ -8550,14 +8558,14 @@
       </c>
     </row>
     <row r="208" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="10">
+      <c r="A208">
         <v>194</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
@@ -8573,10 +8581,10 @@
         <v>195</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
@@ -8592,10 +8600,10 @@
         <v>196</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
@@ -8611,10 +8619,10 @@
         <v>197</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
@@ -8625,8 +8633,27 @@
         <v>57</v>
       </c>
     </row>
+    <row r="212" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>198</v>
+      </c>
+      <c r="B212" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="C212" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="D212" s="14"/>
+      <c r="E212" s="14"/>
+      <c r="F212" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="G212" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A14:J211" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
+  <autoFilter ref="A14:J212" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>

<commit_message>
- Unterstützung für erweiterte iTrassen-Codierung:   - Neue Punktarten: "Messpunkt" (1,2) und "SOK" (1,2)   - Spurweite als neues Attribut für Gleispunkt   - Alternative Attribut-Schreibweisen "-u*" and "-ueb*" (w/o "i")   - Überhöhung und Spurweite werden auch mit NKS erkannt und geschrieben. - InfoText: Angaben für Überhöhung werden auch mit NKS erkannt. - Punktarterkennung jetzt auch von PArtText (KindText)
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7BB1770-AABD-4210-851A-DA3146DAE92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117C7F9-D0F4-42FA-84F2-D17492D942B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3190" yWindow="1820" windowWidth="19540" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$J$212</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$I$213</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="532">
   <si>
     <t>GK.X</t>
   </si>
@@ -1815,9 +1815,6 @@
     <t>Stationsbegleitende Info 9</t>
   </si>
   <si>
-    <t>neu</t>
-  </si>
-  <si>
     <t>Pkt.V.ArtKz.2</t>
   </si>
   <si>
@@ -1836,9 +1833,6 @@
     <t>PktNr</t>
   </si>
   <si>
-    <t>iTC: Vart FP/GVP</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -1891,10 +1885,6 @@
   </si>
   <si>
     <t>Soll</t>
-  </si>
-  <si>
-    <t>iTC: Überhöhung
-Ueb</t>
   </si>
   <si>
     <t>Ist
@@ -2046,6 +2036,25 @@
   </si>
   <si>
     <t>Name Trassenkonfiguration</t>
+  </si>
+  <si>
+    <t>iTC: VArt FP/GVP</t>
+  </si>
+  <si>
+    <t>iTC: (-ueb / -iueb) * -1
+Ueb</t>
+  </si>
+  <si>
+    <t>iTC: -u / -iu</t>
+  </si>
+  <si>
+    <t>Tra.sp</t>
+  </si>
+  <si>
+    <t>Spurweite</t>
+  </si>
+  <si>
+    <t>iTC: -sp</t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2171,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2190,12 +2199,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2435,7 +2438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2569,12 +2572,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4030,18 +4027,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -4184,10 +4181,10 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J212"/>
+  <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105:E107"/>
+    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:XFD116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4200,24 +4197,22 @@
     <col min="6" max="6" width="27.54296875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.453125" customWidth="1"/>
     <col min="8" max="9" width="20.453125" style="46" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="42" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:9" s="42" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="43"/>
       <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-    </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
         <v>394</v>
@@ -4229,9 +4224,8 @@
       <c r="G2" s="30"/>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-    </row>
-    <row r="3" spans="1:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32" t="s">
         <v>141</v>
@@ -4243,9 +4237,8 @@
       <c r="G3" s="36"/>
       <c r="H3" s="45"/>
       <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-    </row>
-    <row r="4" spans="1:10" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
         <v>395</v>
@@ -4257,9 +4250,8 @@
       <c r="G4" s="30"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-    </row>
-    <row r="5" spans="1:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="32" t="s">
         <v>168</v>
@@ -4271,9 +4263,8 @@
       <c r="G5" s="36"/>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-    </row>
-    <row r="6" spans="1:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="32" t="s">
         <v>156</v>
@@ -4285,9 +4276,8 @@
       <c r="G6" s="36"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-    </row>
-    <row r="7" spans="1:10" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26"/>
       <c r="B7" s="27" t="s">
         <v>139</v>
@@ -4299,9 +4289,8 @@
       <c r="G7" s="30"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="32" t="s">
         <v>396</v>
@@ -4313,9 +4302,8 @@
       <c r="G8" s="36"/>
       <c r="H8" s="45"/>
       <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-    </row>
-    <row r="9" spans="1:10" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26"/>
       <c r="B9" s="27" t="s">
         <v>397</v>
@@ -4327,9 +4315,8 @@
       <c r="G9" s="30"/>
       <c r="H9" s="44"/>
       <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-    </row>
-    <row r="10" spans="1:10" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26"/>
       <c r="B10" s="27" t="s">
         <v>169</v>
@@ -4341,9 +4328,8 @@
       <c r="G10" s="30"/>
       <c r="H10" s="44"/>
       <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-    </row>
-    <row r="11" spans="1:10" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>170</v>
@@ -4355,9 +4341,8 @@
       <c r="G11" s="36"/>
       <c r="H11" s="45"/>
       <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-    </row>
-    <row r="12" spans="1:10" s="16" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" s="16" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="38"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -4367,9 +4352,8 @@
       <c r="G12" s="41"/>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-    </row>
-    <row r="13" spans="1:10" s="19" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" ht="22.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>135</v>
       </c>
@@ -4385,21 +4369,18 @@
       <c r="E13" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="60" t="s">
+      <c r="F13" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="61"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="48" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>474</v>
-      </c>
-      <c r="J13" s="53">
-        <v>44257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="25" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="25" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>136</v>
       </c>
@@ -4414,16 +4395,13 @@
         <v>140</v>
       </c>
       <c r="H14" s="49" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I14" s="49" t="s">
-        <v>475</v>
-      </c>
-      <c r="J14" s="52" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="16" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="16" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>1</v>
       </c>
@@ -4443,9 +4421,8 @@
       <c r="G15" s="15"/>
       <c r="H15" s="44"/>
       <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4462,7 +4439,7 @@
       </c>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>3</v>
       </c>
@@ -4479,7 +4456,7 @@
       </c>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4</v>
       </c>
@@ -4496,7 +4473,7 @@
       </c>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>5</v>
       </c>
@@ -4513,7 +4490,7 @@
       </c>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>6</v>
       </c>
@@ -4530,7 +4507,7 @@
       </c>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>7</v>
       </c>
@@ -4547,7 +4524,7 @@
       </c>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>8</v>
       </c>
@@ -4564,7 +4541,7 @@
       </c>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>9</v>
       </c>
@@ -4581,7 +4558,7 @@
       </c>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>10</v>
       </c>
@@ -4598,7 +4575,7 @@
       </c>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>11</v>
       </c>
@@ -4615,13 +4592,13 @@
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="46" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I25" s="46" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>12</v>
       </c>
@@ -4638,7 +4615,7 @@
       </c>
       <c r="G26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>13</v>
       </c>
@@ -4655,7 +4632,7 @@
       </c>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>14</v>
       </c>
@@ -4672,7 +4649,7 @@
       </c>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>15</v>
       </c>
@@ -4691,21 +4668,21 @@
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="46" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I29" s="46" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>16</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -4717,13 +4694,10 @@
         <v>51</v>
       </c>
       <c r="I30" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J30" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>17</v>
       </c>
@@ -4740,13 +4714,13 @@
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="47" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I31" s="46" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>18</v>
       </c>
@@ -4763,13 +4737,13 @@
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="47" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I32" s="46" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <v>19</v>
       </c>
@@ -4786,7 +4760,7 @@
       </c>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>20</v>
       </c>
@@ -4803,7 +4777,7 @@
       </c>
       <c r="G34" s="15"/>
     </row>
-    <row r="35" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>21</v>
       </c>
@@ -4820,7 +4794,7 @@
       </c>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <v>22</v>
       </c>
@@ -4837,7 +4811,7 @@
       </c>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>23</v>
       </c>
@@ -4854,21 +4828,21 @@
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="46" t="s">
-        <v>459</v>
+        <v>526</v>
       </c>
       <c r="I37" s="46" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>24</v>
       </c>
       <c r="B38" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>453</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>454</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -4877,16 +4851,13 @@
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="47" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I38" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J38" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>25</v>
       </c>
@@ -4903,7 +4874,7 @@
       </c>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>26</v>
       </c>
@@ -4920,7 +4891,7 @@
       </c>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>27</v>
       </c>
@@ -4937,7 +4908,7 @@
       </c>
       <c r="G41" s="15"/>
     </row>
-    <row r="42" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>28</v>
       </c>
@@ -4954,7 +4925,7 @@
       </c>
       <c r="G42" s="15"/>
     </row>
-    <row r="43" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>29</v>
       </c>
@@ -4971,7 +4942,7 @@
       </c>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>30</v>
       </c>
@@ -4988,7 +4959,7 @@
       </c>
       <c r="G44" s="15"/>
     </row>
-    <row r="45" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10">
         <v>31</v>
       </c>
@@ -5005,7 +4976,7 @@
       </c>
       <c r="G45" s="15"/>
     </row>
-    <row r="46" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>32</v>
       </c>
@@ -5022,7 +4993,7 @@
       </c>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>33</v>
       </c>
@@ -5039,7 +5010,7 @@
       </c>
       <c r="G47" s="15"/>
     </row>
-    <row r="48" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10">
         <v>34</v>
       </c>
@@ -5430,10 +5401,10 @@
         <v>57</v>
       </c>
       <c r="H68" s="46" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I68" s="46" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5457,10 +5428,10 @@
         <v>57</v>
       </c>
       <c r="H69" s="46" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I69" s="46" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5484,10 +5455,10 @@
         <v>57</v>
       </c>
       <c r="H70" s="46" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I70" s="46" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5700,7 +5671,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10">
         <v>67</v>
       </c>
@@ -5721,7 +5692,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>68</v>
       </c>
@@ -5742,7 +5713,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>69</v>
       </c>
@@ -5765,13 +5736,13 @@
         <v>57</v>
       </c>
       <c r="H83" s="46" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I83" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10">
         <v>70</v>
       </c>
@@ -5794,13 +5765,13 @@
         <v>57</v>
       </c>
       <c r="H84" s="46" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I84" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>71</v>
       </c>
@@ -5819,13 +5790,13 @@
         <v>57</v>
       </c>
       <c r="H85" s="46" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I85" s="51" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>72</v>
       </c>
@@ -5844,13 +5815,13 @@
         <v>57</v>
       </c>
       <c r="H86" s="46" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="I86" s="51" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10">
         <v>73</v>
       </c>
@@ -5869,7 +5840,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>74</v>
       </c>
@@ -5890,13 +5861,13 @@
         <v>57</v>
       </c>
       <c r="H88" s="46" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I88" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>75</v>
       </c>
@@ -5917,7 +5888,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="10">
         <v>76</v>
       </c>
@@ -5938,13 +5909,13 @@
         <v>57</v>
       </c>
       <c r="H90" s="46" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I90" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>77</v>
       </c>
@@ -5965,13 +5936,13 @@
         <v>57</v>
       </c>
       <c r="H91" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I91" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>78</v>
       </c>
@@ -5992,13 +5963,13 @@
         <v>57</v>
       </c>
       <c r="H92" s="46" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I92" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="10">
         <v>79</v>
       </c>
@@ -6019,13 +5990,13 @@
         <v>57</v>
       </c>
       <c r="H93" s="46" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I93" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>80</v>
       </c>
@@ -6046,13 +6017,13 @@
         <v>57</v>
       </c>
       <c r="H94" s="46" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="I94" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>81</v>
       </c>
@@ -6073,13 +6044,13 @@
         <v>57</v>
       </c>
       <c r="H95" s="46" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I95" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10">
         <v>82</v>
       </c>
@@ -6100,16 +6071,13 @@
         <v>57</v>
       </c>
       <c r="H96" s="46" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I96" s="46" t="s">
-        <v>476</v>
-      </c>
-      <c r="J96" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>83</v>
       </c>
@@ -6130,16 +6098,13 @@
         <v>57</v>
       </c>
       <c r="H97" s="46" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I97" s="46" t="s">
-        <v>476</v>
-      </c>
-      <c r="J97" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>84</v>
       </c>
@@ -6160,13 +6125,13 @@
         <v>57</v>
       </c>
       <c r="H98" s="46" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I98" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10">
         <v>85</v>
       </c>
@@ -6187,13 +6152,13 @@
         <v>57</v>
       </c>
       <c r="H99" s="46" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I99" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>86</v>
       </c>
@@ -6214,13 +6179,13 @@
         <v>57</v>
       </c>
       <c r="H100" s="46" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I100" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>87</v>
       </c>
@@ -6241,13 +6206,13 @@
         <v>57</v>
       </c>
       <c r="H101" s="46" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I101" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10">
         <v>88</v>
       </c>
@@ -6268,13 +6233,13 @@
         <v>57</v>
       </c>
       <c r="H102" s="46" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I102" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>89</v>
       </c>
@@ -6295,13 +6260,13 @@
         <v>57</v>
       </c>
       <c r="H103" s="46" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I103" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>90</v>
       </c>
@@ -6322,21 +6287,21 @@
         <v>57</v>
       </c>
       <c r="H104" s="46" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I104" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10">
         <v>91</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -6347,7 +6312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>92</v>
       </c>
@@ -6366,7 +6331,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>93</v>
       </c>
@@ -6378,7 +6343,7 @@
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F107" s="14" t="s">
         <v>25</v>
@@ -6387,7 +6352,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="10">
         <v>94</v>
       </c>
@@ -6406,7 +6371,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>95</v>
       </c>
@@ -6425,7 +6390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>96</v>
       </c>
@@ -6444,7 +6409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10">
         <v>97</v>
       </c>
@@ -6463,7 +6428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>98</v>
       </c>
@@ -6482,7 +6447,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>99</v>
       </c>
@@ -6501,7 +6466,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10">
         <v>100</v>
       </c>
@@ -6522,13 +6487,13 @@
         <v>57</v>
       </c>
       <c r="H114" s="46" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I114" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>101</v>
       </c>
@@ -6549,21 +6514,21 @@
         <v>57</v>
       </c>
       <c r="H115" s="46" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I115" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>102</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>20</v>
+        <v>529</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>330</v>
+        <v>530</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>44</v>
@@ -6576,22 +6541,21 @@
         <v>57</v>
       </c>
       <c r="H116" s="50" t="s">
-        <v>478</v>
+        <v>531</v>
       </c>
       <c r="I116" s="50" t="s">
-        <v>479</v>
-      </c>
-      <c r="J116" s="50"/>
-    </row>
-    <row r="117" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="10">
         <v>103</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>332</v>
+        <v>20</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>44</v>
@@ -6603,16 +6567,22 @@
       <c r="G117" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H117" s="50" t="s">
+        <v>528</v>
+      </c>
+      <c r="I117" s="50" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>104</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>430</v>
+        <v>332</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>431</v>
+        <v>331</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>44</v>
@@ -6624,25 +6594,22 @@
       <c r="G118" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H118" s="46" t="s">
-        <v>471</v>
-      </c>
-      <c r="I118" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J118" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H118" s="50" t="s">
+        <v>527</v>
+      </c>
+      <c r="I118" s="50" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>105</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D119" s="14" t="s">
         <v>44</v>
@@ -6655,24 +6622,21 @@
         <v>57</v>
       </c>
       <c r="H119" s="46" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I119" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J119" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="10">
         <v>106</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>19</v>
+        <v>432</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="D120" s="14" t="s">
         <v>44</v>
@@ -6685,21 +6649,21 @@
         <v>57</v>
       </c>
       <c r="H120" s="46" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="I120" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>107</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>420</v>
+        <v>19</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D121" s="14" t="s">
         <v>44</v>
@@ -6712,24 +6676,21 @@
         <v>57</v>
       </c>
       <c r="H121" s="46" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I121" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J121" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>108</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>38</v>
+        <v>420</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>27</v>
+        <v>421</v>
       </c>
       <c r="D122" s="14" t="s">
         <v>44</v>
@@ -6742,24 +6703,24 @@
         <v>57</v>
       </c>
       <c r="H122" s="46" t="s">
-        <v>480</v>
+        <v>495</v>
       </c>
       <c r="I122" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="10">
         <v>109</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>408</v>
+        <v>38</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>409</v>
+        <v>27</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E123" s="14"/>
       <c r="F123" s="14" t="s">
@@ -6769,24 +6730,24 @@
         <v>57</v>
       </c>
       <c r="H123" s="46" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="I123" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>110</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>385</v>
+        <v>409</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E124" s="14"/>
       <c r="F124" s="14" t="s">
@@ -6796,21 +6757,21 @@
         <v>57</v>
       </c>
       <c r="H124" s="46" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="I124" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>111</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D125" s="14" t="s">
         <v>44</v>
@@ -6823,23 +6784,25 @@
         <v>57</v>
       </c>
       <c r="H125" s="46" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="I125" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="10">
         <v>112</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="D126" s="14"/>
+        <v>384</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E126" s="14"/>
       <c r="F126" s="14" t="s">
         <v>25</v>
@@ -6847,20 +6810,24 @@
       <c r="G126" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H126" s="46" t="s">
+        <v>480</v>
+      </c>
+      <c r="I126" s="46" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>113</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="D127" s="14"/>
       <c r="E127" s="14"/>
       <c r="F127" s="14" t="s">
         <v>25</v>
@@ -6869,15 +6836,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>114</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>411</v>
+        <v>370</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>412</v>
+        <v>371</v>
       </c>
       <c r="D128" s="14" t="s">
         <v>44</v>
@@ -6889,25 +6856,16 @@
       <c r="G128" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H128" s="46" t="s">
-        <v>504</v>
-      </c>
-      <c r="I128" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J128" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="10">
         <v>115</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>44</v>
@@ -6920,24 +6878,21 @@
         <v>57</v>
       </c>
       <c r="H129" s="46" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I129" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J129" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>116</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>44</v>
@@ -6950,24 +6905,21 @@
         <v>57</v>
       </c>
       <c r="H130" s="46" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I130" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J130" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>117</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>44</v>
@@ -6980,24 +6932,21 @@
         <v>57</v>
       </c>
       <c r="H131" s="46" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I131" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J131" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="10">
         <v>118</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D132" s="14" t="s">
         <v>44</v>
@@ -7010,26 +6959,25 @@
         <v>57</v>
       </c>
       <c r="H132" s="46" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I132" s="46" t="s">
-        <v>477</v>
-      </c>
-      <c r="J132" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>119</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="D133" s="14"/>
+        <v>418</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E133" s="14"/>
       <c r="F133" s="14" t="s">
         <v>25</v>
@@ -7038,24 +6986,21 @@
         <v>57</v>
       </c>
       <c r="H133" s="46" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="I133" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J133" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>120</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
@@ -7066,24 +7011,21 @@
         <v>57</v>
       </c>
       <c r="H134" s="46" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I134" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J134" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="10">
         <v>121</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
@@ -7094,24 +7036,21 @@
         <v>57</v>
       </c>
       <c r="H135" s="46" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I135" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J135" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>122</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
@@ -7122,24 +7061,21 @@
         <v>57</v>
       </c>
       <c r="H136" s="46" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I136" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J136" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>123</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
@@ -7150,24 +7086,21 @@
         <v>57</v>
       </c>
       <c r="H137" s="46" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="I137" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J137" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="10">
         <v>124</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
@@ -7178,24 +7111,21 @@
         <v>57</v>
       </c>
       <c r="H138" s="46" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I138" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J138" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>125</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
@@ -7206,24 +7136,21 @@
         <v>57</v>
       </c>
       <c r="H139" s="46" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I139" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J139" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>126</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
@@ -7234,24 +7161,21 @@
         <v>57</v>
       </c>
       <c r="H140" s="46" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I140" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J140" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="10">
         <v>127</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
@@ -7262,51 +7186,46 @@
         <v>57</v>
       </c>
       <c r="H141" s="46" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="I141" s="46" t="s">
-        <v>503</v>
-      </c>
-      <c r="J141" s="46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>128</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>250</v>
+        <v>443</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="D142" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="D142" s="14"/>
       <c r="E142" s="14"/>
       <c r="F142" s="14" t="s">
-        <v>254</v>
+        <v>25</v>
       </c>
       <c r="G142" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H142" s="46" t="s">
-        <v>491</v>
+        <v>514</v>
       </c>
       <c r="I142" s="46" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>129</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D143" s="14" t="s">
         <v>44</v>
@@ -7319,23 +7238,25 @@
         <v>57</v>
       </c>
       <c r="H143" s="46" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I143" s="46" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="10">
         <v>130</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D144" s="14"/>
+        <v>253</v>
+      </c>
+      <c r="D144" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E144" s="14"/>
       <c r="F144" s="14" t="s">
         <v>254</v>
@@ -7343,21 +7264,27 @@
       <c r="G144" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="H144" s="46" t="s">
+        <v>489</v>
+      </c>
+      <c r="I144" s="46" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="145" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>131</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
       <c r="F145" s="14" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="G145" s="15" t="s">
         <v>57</v>
@@ -7368,10 +7295,10 @@
         <v>132</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
@@ -7387,10 +7314,10 @@
         <v>133</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
@@ -7406,10 +7333,10 @@
         <v>134</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
@@ -7425,10 +7352,10 @@
         <v>135</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
@@ -7444,10 +7371,10 @@
         <v>136</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
@@ -7463,10 +7390,10 @@
         <v>137</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
@@ -7482,14 +7409,12 @@
         <v>138</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D152" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D152" s="14"/>
       <c r="E152" s="14"/>
       <c r="F152" s="14" t="s">
         <v>218</v>
@@ -7503,12 +7428,14 @@
         <v>139</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="D153" s="14"/>
+        <v>215</v>
+      </c>
+      <c r="D153" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="E153" s="14"/>
       <c r="F153" s="14" t="s">
         <v>218</v>
@@ -7522,10 +7449,10 @@
         <v>140</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
@@ -7541,10 +7468,10 @@
         <v>141</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
@@ -7560,10 +7487,10 @@
         <v>142</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
@@ -7579,10 +7506,10 @@
         <v>143</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
@@ -7598,10 +7525,10 @@
         <v>144</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
@@ -7617,10 +7544,10 @@
         <v>145</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
@@ -7636,10 +7563,10 @@
         <v>146</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
@@ -7655,10 +7582,10 @@
         <v>147</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
@@ -7674,14 +7601,12 @@
         <v>148</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D162" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D162" s="14"/>
       <c r="E162" s="14"/>
       <c r="F162" s="14" t="s">
         <v>218</v>
@@ -7695,12 +7620,14 @@
         <v>149</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="D163" s="14"/>
+        <v>233</v>
+      </c>
+      <c r="D163" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E163" s="14"/>
       <c r="F163" s="14" t="s">
         <v>218</v>
@@ -7714,10 +7641,10 @@
         <v>150</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
@@ -7733,10 +7660,10 @@
         <v>151</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
@@ -7752,10 +7679,10 @@
         <v>152</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
@@ -7771,10 +7698,10 @@
         <v>153</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
@@ -7790,10 +7717,10 @@
         <v>154</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
@@ -7809,15 +7736,15 @@
         <v>155</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
       <c r="F169" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G169" s="15" t="s">
         <v>57</v>
@@ -7828,14 +7755,12 @@
         <v>156</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D170" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D170" s="14"/>
       <c r="E170" s="14"/>
       <c r="F170" s="14" t="s">
         <v>217</v>
@@ -7849,12 +7774,14 @@
         <v>157</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D171" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="D171" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E171" s="14"/>
       <c r="F171" s="14" t="s">
         <v>217</v>
@@ -7868,10 +7795,10 @@
         <v>158</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
@@ -7887,14 +7814,12 @@
         <v>159</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>301</v>
+        <v>186</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="D173" s="14"/>
       <c r="E173" s="14"/>
       <c r="F173" s="14" t="s">
         <v>217</v>
@@ -7908,15 +7833,17 @@
         <v>160</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="D174" s="14"/>
+        <v>302</v>
+      </c>
+      <c r="D174" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E174" s="14"/>
       <c r="F174" s="14" t="s">
-        <v>313</v>
+        <v>217</v>
       </c>
       <c r="G174" s="15" t="s">
         <v>57</v>
@@ -7927,10 +7854,10 @@
         <v>161</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
@@ -7946,10 +7873,10 @@
         <v>162</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
@@ -7965,10 +7892,10 @@
         <v>163</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
@@ -7984,10 +7911,10 @@
         <v>164</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
@@ -8003,10 +7930,10 @@
         <v>165</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
@@ -8022,10 +7949,10 @@
         <v>166</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
@@ -8041,10 +7968,10 @@
         <v>167</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
@@ -8060,15 +7987,15 @@
         <v>168</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
       <c r="F182" s="14" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="G182" s="15" t="s">
         <v>57</v>
@@ -8079,10 +8006,10 @@
         <v>169</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>377</v>
+        <v>342</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>378</v>
+        <v>339</v>
       </c>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
@@ -8098,10 +8025,10 @@
         <v>170</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
@@ -8117,10 +8044,10 @@
         <v>171</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
@@ -8136,10 +8063,10 @@
         <v>172</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>526</v>
+        <v>340</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>521</v>
+        <v>337</v>
       </c>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
@@ -8155,10 +8082,10 @@
         <v>173</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C187" s="14" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
@@ -8174,10 +8101,10 @@
         <v>174</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C188" s="14" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
@@ -8193,10 +8120,10 @@
         <v>175</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>341</v>
+        <v>521</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>338</v>
+        <v>522</v>
       </c>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
@@ -8212,10 +8139,10 @@
         <v>176</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C190" s="14" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
@@ -8231,10 +8158,10 @@
         <v>177</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
@@ -8250,10 +8177,10 @@
         <v>178</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
@@ -8269,10 +8196,10 @@
         <v>179</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
@@ -8288,15 +8215,15 @@
         <v>180</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
       <c r="F194" s="14" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G194" s="15" t="s">
         <v>57</v>
@@ -8307,10 +8234,10 @@
         <v>181</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
@@ -8326,10 +8253,10 @@
         <v>182</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
@@ -8345,14 +8272,12 @@
         <v>183</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="D197" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="D197" s="14"/>
       <c r="E197" s="14"/>
       <c r="F197" s="14" t="s">
         <v>335</v>
@@ -8366,10 +8291,10 @@
         <v>184</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D198" s="14" t="s">
         <v>44</v>
@@ -8387,10 +8312,10 @@
         <v>185</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D199" s="14" t="s">
         <v>44</v>
@@ -8408,10 +8333,10 @@
         <v>186</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>44</v>
@@ -8429,12 +8354,14 @@
         <v>187</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="D201" s="14"/>
+        <v>361</v>
+      </c>
+      <c r="D201" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E201" s="14"/>
       <c r="F201" s="14" t="s">
         <v>335</v>
@@ -8448,10 +8375,10 @@
         <v>188</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
@@ -8467,10 +8394,10 @@
         <v>189</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
@@ -8486,10 +8413,10 @@
         <v>190</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>373</v>
+        <v>400</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>375</v>
+        <v>401</v>
       </c>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
@@ -8505,10 +8432,10 @@
         <v>191</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
@@ -8524,10 +8451,10 @@
         <v>192</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
@@ -8543,10 +8470,10 @@
         <v>193</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
@@ -8562,10 +8489,10 @@
         <v>194</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
@@ -8581,10 +8508,10 @@
         <v>195</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
@@ -8600,10 +8527,10 @@
         <v>196</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
@@ -8619,10 +8546,10 @@
         <v>197</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
@@ -8638,10 +8565,10 @@
         <v>198</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C212" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
@@ -8652,8 +8579,27 @@
         <v>57</v>
       </c>
     </row>
+    <row r="213" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A213" s="10">
+        <v>199</v>
+      </c>
+      <c r="B213" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="C213" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="D213" s="14"/>
+      <c r="E213" s="14"/>
+      <c r="F213" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="G213" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A14:J212" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
+  <autoFilter ref="A14:I213" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>

<commit_message>
- CimpTrassenkoo: Bugfix: iGeo-Trassennamen mit "." werden nicht mehr verstümmelt. - CtabAktiveTabelle.Syncronisieren() setzt jetzt auch Arbeitsverzeichnis.
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117C7F9-D0F4-42FA-84F2-D17492D942B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B3AA43-8441-46C5-A3DF-EE777A384BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$I$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$I$212</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -1023,9 +1023,6 @@
     <t>CAD-Symbol Rotation</t>
   </si>
   <si>
-    <t>CAD-Element Ebene</t>
-  </si>
-  <si>
     <t>Kodierung</t>
   </si>
   <si>
@@ -1066,9 +1063,6 @@
   </si>
   <si>
     <t>CAD.Attr.Dicke</t>
-  </si>
-  <si>
-    <t>###CAD.Attr.Lv</t>
   </si>
   <si>
     <t>CAD-Element ID</t>
@@ -2055,6 +2049,12 @@
   </si>
   <si>
     <t>iTC: -sp</t>
+  </si>
+  <si>
+    <t>LRP.GeometrieTrend</t>
+  </si>
+  <si>
+    <t>LRP GeometrieTrend (k = konstant, v = variabel, ? = unbekannt)</t>
   </si>
 </sst>
 </file>
@@ -4013,7 +4013,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -4056,10 +4056,10 @@
         <v>155</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4092,7 +4092,7 @@
         <v>167</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4183,8 +4183,8 @@
   </sheetPr>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116:XFD116"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4215,7 +4215,7 @@
     <row r="2" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26"/>
       <c r="B2" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="27"/>
@@ -4241,7 +4241,7 @@
     <row r="4" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="26"/>
       <c r="B4" s="27" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="27"/>
@@ -4293,7 +4293,7 @@
     <row r="8" spans="1:9" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
@@ -4306,7 +4306,7 @@
     <row r="9" spans="1:9" s="16" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26"/>
       <c r="B9" s="27" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="27"/>
@@ -4374,10 +4374,10 @@
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="48" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="25" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4395,10 +4395,10 @@
         <v>140</v>
       </c>
       <c r="H14" s="49" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I14" s="49" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
@@ -4592,10 +4592,10 @@
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="46" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I25" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4668,10 +4668,10 @@
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="46" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I29" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4679,10 +4679,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -4694,7 +4694,7 @@
         <v>51</v>
       </c>
       <c r="I30" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4714,10 +4714,10 @@
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="47" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I31" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4737,10 +4737,10 @@
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="47" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="I32" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4828,10 +4828,10 @@
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="46" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I37" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4839,10 +4839,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -4851,10 +4851,10 @@
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="47" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I38" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4930,10 +4930,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -4947,10 +4947,10 @@
         <v>30</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -4964,10 +4964,10 @@
         <v>31</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -4981,10 +4981,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
@@ -4998,10 +4998,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
@@ -5015,10 +5015,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -5032,10 +5032,10 @@
         <v>35</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
@@ -5049,10 +5049,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
@@ -5066,10 +5066,10 @@
         <v>37</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -5083,10 +5083,10 @@
         <v>38</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
@@ -5271,10 +5271,10 @@
         <v>48</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
@@ -5290,10 +5290,10 @@
         <v>49</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
@@ -5309,10 +5309,10 @@
         <v>50</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
@@ -5328,7 +5328,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>84</v>
@@ -5347,7 +5347,7 @@
         <v>52</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>83</v>
@@ -5366,10 +5366,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
@@ -5401,10 +5401,10 @@
         <v>57</v>
       </c>
       <c r="H68" s="46" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I68" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5428,10 +5428,10 @@
         <v>57</v>
       </c>
       <c r="H69" s="46" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I69" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5455,10 +5455,10 @@
         <v>57</v>
       </c>
       <c r="H70" s="46" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I70" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5736,10 +5736,10 @@
         <v>57</v>
       </c>
       <c r="H83" s="46" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I83" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5765,10 +5765,10 @@
         <v>57</v>
       </c>
       <c r="H84" s="46" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I84" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5776,10 +5776,10 @@
         <v>71</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
@@ -5790,10 +5790,10 @@
         <v>57</v>
       </c>
       <c r="H85" s="46" t="s">
+        <v>496</v>
+      </c>
+      <c r="I85" s="51" t="s">
         <v>498</v>
-      </c>
-      <c r="I85" s="51" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5801,10 +5801,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
@@ -5815,10 +5815,10 @@
         <v>57</v>
       </c>
       <c r="H86" s="46" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I86" s="51" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5826,10 +5826,10 @@
         <v>73</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
@@ -5861,10 +5861,10 @@
         <v>57</v>
       </c>
       <c r="H88" s="46" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I88" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5896,7 +5896,7 @@
         <v>5</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D90" s="14" t="s">
         <v>44</v>
@@ -5909,10 +5909,10 @@
         <v>57</v>
       </c>
       <c r="H90" s="46" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I90" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5936,10 +5936,10 @@
         <v>57</v>
       </c>
       <c r="H91" s="46" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I91" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5963,10 +5963,10 @@
         <v>57</v>
       </c>
       <c r="H92" s="46" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I92" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5977,7 +5977,7 @@
         <v>4</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D93" s="14" t="s">
         <v>44</v>
@@ -5990,10 +5990,10 @@
         <v>57</v>
       </c>
       <c r="H93" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I93" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6001,10 +6001,10 @@
         <v>80</v>
       </c>
       <c r="B94" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C94" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>267</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>44</v>
@@ -6017,10 +6017,10 @@
         <v>57</v>
       </c>
       <c r="H94" s="46" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I94" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6028,10 +6028,10 @@
         <v>81</v>
       </c>
       <c r="B95" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C95" s="14" t="s">
         <v>266</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>268</v>
       </c>
       <c r="D95" s="14" t="s">
         <v>44</v>
@@ -6044,10 +6044,10 @@
         <v>57</v>
       </c>
       <c r="H95" s="46" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I95" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6055,10 +6055,10 @@
         <v>82</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D96" s="14" t="s">
         <v>44</v>
@@ -6071,10 +6071,10 @@
         <v>57</v>
       </c>
       <c r="H96" s="46" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I96" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6082,10 +6082,10 @@
         <v>83</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D97" s="14" t="s">
         <v>44</v>
@@ -6098,10 +6098,10 @@
         <v>57</v>
       </c>
       <c r="H97" s="46" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I97" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6109,10 +6109,10 @@
         <v>84</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D98" s="14" t="s">
         <v>44</v>
@@ -6125,10 +6125,10 @@
         <v>57</v>
       </c>
       <c r="H98" s="46" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I98" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6136,10 +6136,10 @@
         <v>85</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D99" s="14" t="s">
         <v>44</v>
@@ -6152,10 +6152,10 @@
         <v>57</v>
       </c>
       <c r="H99" s="46" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I99" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6179,10 +6179,10 @@
         <v>57</v>
       </c>
       <c r="H100" s="46" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I100" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6206,10 +6206,10 @@
         <v>57</v>
       </c>
       <c r="H101" s="46" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I101" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6217,10 +6217,10 @@
         <v>88</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>44</v>
@@ -6233,10 +6233,10 @@
         <v>57</v>
       </c>
       <c r="H102" s="46" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I102" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6244,10 +6244,10 @@
         <v>89</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>44</v>
@@ -6260,10 +6260,10 @@
         <v>57</v>
       </c>
       <c r="H103" s="46" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I103" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6274,7 +6274,7 @@
         <v>12</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>44</v>
@@ -6287,10 +6287,10 @@
         <v>57</v>
       </c>
       <c r="H104" s="46" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I104" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6298,10 +6298,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="14"/>
@@ -6343,7 +6343,7 @@
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="14" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F107" s="14" t="s">
         <v>25</v>
@@ -6398,7 +6398,7 @@
         <v>159</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
@@ -6417,7 +6417,7 @@
         <v>160</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D111" s="14"/>
       <c r="E111" s="14"/>
@@ -6433,10 +6433,10 @@
         <v>98</v>
       </c>
       <c r="B112" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>261</v>
       </c>
       <c r="D112" s="14"/>
       <c r="E112" s="14"/>
@@ -6452,10 +6452,10 @@
         <v>99</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
@@ -6487,10 +6487,10 @@
         <v>57</v>
       </c>
       <c r="H114" s="46" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I114" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6514,10 +6514,10 @@
         <v>57</v>
       </c>
       <c r="H115" s="46" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I115" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -6525,10 +6525,10 @@
         <v>102</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>44</v>
@@ -6541,10 +6541,10 @@
         <v>57</v>
       </c>
       <c r="H116" s="50" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I116" s="50" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -6555,7 +6555,7 @@
         <v>20</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>44</v>
@@ -6568,10 +6568,10 @@
         <v>57</v>
       </c>
       <c r="H117" s="50" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I117" s="50" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="26" x14ac:dyDescent="0.35">
@@ -6579,10 +6579,10 @@
         <v>104</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>44</v>
@@ -6595,10 +6595,10 @@
         <v>57</v>
       </c>
       <c r="H118" s="50" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="I118" s="50" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6606,10 +6606,10 @@
         <v>105</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D119" s="14" t="s">
         <v>44</v>
@@ -6622,10 +6622,10 @@
         <v>57</v>
       </c>
       <c r="H119" s="46" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I119" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6633,10 +6633,10 @@
         <v>106</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D120" s="14" t="s">
         <v>44</v>
@@ -6649,10 +6649,10 @@
         <v>57</v>
       </c>
       <c r="H120" s="46" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I120" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6663,7 +6663,7 @@
         <v>19</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D121" s="14" t="s">
         <v>44</v>
@@ -6676,10 +6676,10 @@
         <v>57</v>
       </c>
       <c r="H121" s="46" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I121" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6687,10 +6687,10 @@
         <v>108</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D122" s="14" t="s">
         <v>44</v>
@@ -6703,10 +6703,10 @@
         <v>57</v>
       </c>
       <c r="H122" s="46" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I122" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6730,10 +6730,10 @@
         <v>57</v>
       </c>
       <c r="H123" s="46" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I123" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6741,10 +6741,10 @@
         <v>110</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D124" s="14" t="s">
         <v>45</v>
@@ -6757,10 +6757,10 @@
         <v>57</v>
       </c>
       <c r="H124" s="46" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I124" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6768,10 +6768,10 @@
         <v>111</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D125" s="14" t="s">
         <v>44</v>
@@ -6784,10 +6784,10 @@
         <v>57</v>
       </c>
       <c r="H125" s="46" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I125" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6795,10 +6795,10 @@
         <v>112</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D126" s="14" t="s">
         <v>44</v>
@@ -6811,10 +6811,10 @@
         <v>57</v>
       </c>
       <c r="H126" s="46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I126" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6822,10 +6822,10 @@
         <v>113</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D127" s="14"/>
       <c r="E127" s="14"/>
@@ -6841,10 +6841,10 @@
         <v>114</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D128" s="14" t="s">
         <v>44</v>
@@ -6862,10 +6862,10 @@
         <v>115</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>44</v>
@@ -6878,10 +6878,10 @@
         <v>57</v>
       </c>
       <c r="H129" s="46" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I129" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6889,10 +6889,10 @@
         <v>116</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>44</v>
@@ -6905,10 +6905,10 @@
         <v>57</v>
       </c>
       <c r="H130" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I130" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6916,10 +6916,10 @@
         <v>117</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>44</v>
@@ -6932,10 +6932,10 @@
         <v>57</v>
       </c>
       <c r="H131" s="46" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I131" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6943,10 +6943,10 @@
         <v>118</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D132" s="14" t="s">
         <v>44</v>
@@ -6959,10 +6959,10 @@
         <v>57</v>
       </c>
       <c r="H132" s="46" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I132" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6970,10 +6970,10 @@
         <v>119</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D133" s="14" t="s">
         <v>44</v>
@@ -6986,10 +6986,10 @@
         <v>57</v>
       </c>
       <c r="H133" s="46" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I133" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6997,10 +6997,10 @@
         <v>120</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D134" s="14"/>
       <c r="E134" s="14"/>
@@ -7011,10 +7011,10 @@
         <v>57</v>
       </c>
       <c r="H134" s="46" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I134" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7022,10 +7022,10 @@
         <v>121</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
@@ -7036,10 +7036,10 @@
         <v>57</v>
       </c>
       <c r="H135" s="46" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I135" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7047,10 +7047,10 @@
         <v>122</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
@@ -7061,10 +7061,10 @@
         <v>57</v>
       </c>
       <c r="H136" s="46" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I136" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7072,10 +7072,10 @@
         <v>123</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
@@ -7086,10 +7086,10 @@
         <v>57</v>
       </c>
       <c r="H137" s="46" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I137" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7097,10 +7097,10 @@
         <v>124</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
@@ -7111,10 +7111,10 @@
         <v>57</v>
       </c>
       <c r="H138" s="46" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I138" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7122,10 +7122,10 @@
         <v>125</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
@@ -7136,10 +7136,10 @@
         <v>57</v>
       </c>
       <c r="H139" s="46" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I139" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7147,10 +7147,10 @@
         <v>126</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
@@ -7161,10 +7161,10 @@
         <v>57</v>
       </c>
       <c r="H140" s="46" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I140" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7172,10 +7172,10 @@
         <v>127</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
@@ -7186,10 +7186,10 @@
         <v>57</v>
       </c>
       <c r="H141" s="46" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I141" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7197,10 +7197,10 @@
         <v>128</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
@@ -7211,10 +7211,10 @@
         <v>57</v>
       </c>
       <c r="H142" s="46" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I142" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7222,26 +7222,26 @@
         <v>129</v>
       </c>
       <c r="B143" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C143" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="C143" s="14" t="s">
-        <v>252</v>
       </c>
       <c r="D143" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E143" s="14"/>
       <c r="F143" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G143" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H143" s="46" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I143" s="46" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7249,26 +7249,26 @@
         <v>130</v>
       </c>
       <c r="B144" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="C144" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="C144" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E144" s="14"/>
       <c r="F144" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G144" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H144" s="46" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I144" s="46" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7276,15 +7276,15 @@
         <v>131</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D145" s="14"/>
       <c r="E145" s="14"/>
       <c r="F145" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G145" s="15" t="s">
         <v>57</v>
@@ -7303,7 +7303,7 @@
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
       <c r="F146" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G146" s="15" t="s">
         <v>57</v>
@@ -7322,26 +7322,26 @@
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
       <c r="F147" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="G147" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="10">
+        <v>134</v>
+      </c>
+      <c r="B148" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G147" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148">
-        <v>134</v>
-      </c>
-      <c r="B148" s="13" t="s">
-        <v>231</v>
-      </c>
       <c r="C148" s="14" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
       <c r="F148" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G148" s="15" t="s">
         <v>57</v>
@@ -7352,93 +7352,93 @@
         <v>135</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
       <c r="F149" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G149" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="10">
+      <c r="A150">
         <v>136</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
       <c r="F150" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G150" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151">
+      <c r="A151" s="10">
         <v>137</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
       <c r="F151" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G151" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152">
+      <c r="A152" s="10">
         <v>138</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D152" s="14"/>
+        <v>215</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="E152" s="14"/>
       <c r="F152" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G152" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="10">
+      <c r="A153">
         <v>139</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D153" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="D153" s="14"/>
       <c r="E153" s="14"/>
       <c r="F153" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G153" s="15" t="s">
         <v>57</v>
@@ -7449,34 +7449,34 @@
         <v>140</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
       <c r="F154" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G154" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155">
+      <c r="A155" s="10">
         <v>141</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
       <c r="F155" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G155" s="15" t="s">
         <v>57</v>
@@ -7490,12 +7490,12 @@
         <v>223</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
       <c r="F156" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G156" s="15" t="s">
         <v>57</v>
@@ -7509,12 +7509,12 @@
         <v>224</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
       <c r="F157" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G157" s="15" t="s">
         <v>57</v>
@@ -7528,12 +7528,12 @@
         <v>225</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
       <c r="F158" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G158" s="15" t="s">
         <v>57</v>
@@ -7544,34 +7544,34 @@
         <v>145</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
       <c r="F159" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G159" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160">
+      <c r="A160" s="10">
         <v>146</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
       <c r="F160" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G160" s="15" t="s">
         <v>57</v>
@@ -7582,93 +7582,93 @@
         <v>147</v>
       </c>
       <c r="B161" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C161" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="C161" s="14" t="s">
-        <v>247</v>
       </c>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
       <c r="F161" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G161" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="10">
+      <c r="A162">
         <v>148</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="D162" s="14"/>
+        <v>231</v>
+      </c>
+      <c r="D162" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E162" s="14"/>
       <c r="F162" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G162" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163">
+      <c r="A163" s="10">
         <v>149</v>
       </c>
       <c r="B163" s="13" t="s">
         <v>227</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D163" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="D163" s="14"/>
       <c r="E163" s="14"/>
       <c r="F163" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G163" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164">
+      <c r="A164" s="10">
         <v>150</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
       <c r="F164" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G164" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="10">
+      <c r="A165">
         <v>151</v>
       </c>
       <c r="B165" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C165" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="C165" s="14" t="s">
-        <v>246</v>
       </c>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
       <c r="F165" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G165" s="15" t="s">
         <v>57</v>
@@ -7679,34 +7679,34 @@
         <v>152</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
       <c r="F166" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G166" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167">
+      <c r="A167" s="10">
         <v>153</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
       <c r="F167" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G167" s="15" t="s">
         <v>57</v>
@@ -7717,15 +7717,15 @@
         <v>154</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
       <c r="F168" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G168" s="15" t="s">
         <v>57</v>
@@ -7736,15 +7736,15 @@
         <v>155</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
       <c r="F169" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G169" s="15" t="s">
         <v>57</v>
@@ -7755,15 +7755,17 @@
         <v>156</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D170" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="D170" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E170" s="14"/>
       <c r="F170" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G170" s="15" t="s">
         <v>57</v>
@@ -7774,36 +7776,34 @@
         <v>157</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D171" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D171" s="14"/>
       <c r="E171" s="14"/>
       <c r="F171" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G171" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172">
+      <c r="A172" s="10">
         <v>158</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
       <c r="F172" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G172" s="15" t="s">
         <v>57</v>
@@ -7814,93 +7814,93 @@
         <v>159</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>186</v>
+        <v>299</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D173" s="14"/>
+        <v>300</v>
+      </c>
+      <c r="D173" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E173" s="14"/>
       <c r="F173" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G173" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="10">
+      <c r="A174">
         <v>160</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="D174" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="D174" s="14"/>
       <c r="E174" s="14"/>
       <c r="F174" s="14" t="s">
-        <v>217</v>
+        <v>311</v>
       </c>
       <c r="G174" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175">
+      <c r="A175" s="10">
         <v>161</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
       <c r="F175" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G175" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176">
+      <c r="A176" s="10">
         <v>162</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
       <c r="F176" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G176" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="10">
+      <c r="A177">
         <v>163</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
       <c r="F177" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G177" s="15" t="s">
         <v>57</v>
@@ -7911,34 +7911,34 @@
         <v>164</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
       <c r="F178" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G178" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179">
+      <c r="A179" s="10">
         <v>165</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
       <c r="F179" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G179" s="15" t="s">
         <v>57</v>
@@ -7949,15 +7949,15 @@
         <v>166</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
       <c r="F180" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G180" s="15" t="s">
         <v>57</v>
@@ -7968,15 +7968,15 @@
         <v>167</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
       <c r="F181" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G181" s="15" t="s">
         <v>57</v>
@@ -7987,15 +7987,15 @@
         <v>168</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
       <c r="F182" s="14" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="G182" s="15" t="s">
         <v>57</v>
@@ -8006,34 +8006,34 @@
         <v>169</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>342</v>
+        <v>375</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>339</v>
+        <v>376</v>
       </c>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
       <c r="F183" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G183" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184">
+      <c r="A184" s="10">
         <v>170</v>
       </c>
       <c r="B184" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="C184" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="C184" s="14" t="s">
-        <v>378</v>
       </c>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
       <c r="F184" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G184" s="15" t="s">
         <v>57</v>
@@ -8044,45 +8044,45 @@
         <v>171</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>380</v>
+        <v>338</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>379</v>
+        <v>335</v>
       </c>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
       <c r="F185" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G185" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="10">
+      <c r="A186">
         <v>172</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>340</v>
+        <v>521</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>337</v>
+        <v>516</v>
       </c>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
       <c r="F186" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G186" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187">
+      <c r="A187" s="10">
         <v>173</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C187" s="14" t="s">
         <v>518</v>
@@ -8090,14 +8090,14 @@
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
       <c r="F187" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G187" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188">
+      <c r="A188" s="10">
         <v>174</v>
       </c>
       <c r="B188" s="13" t="s">
@@ -8109,26 +8109,26 @@
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
       <c r="F188" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G188" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>175</v>
+      </c>
+      <c r="B189" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C189" s="14" t="s">
         <v>336</v>
-      </c>
-      <c r="G188" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="10">
-        <v>175</v>
-      </c>
-      <c r="B189" s="13" t="s">
-        <v>521</v>
-      </c>
-      <c r="C189" s="14" t="s">
-        <v>522</v>
       </c>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
       <c r="F189" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G189" s="15" t="s">
         <v>57</v>
@@ -8139,34 +8139,34 @@
         <v>176</v>
       </c>
       <c r="B190" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C190" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="C190" s="14" t="s">
-        <v>338</v>
       </c>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
       <c r="F190" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G190" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191">
+      <c r="A191" s="10">
         <v>177</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
       <c r="F191" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G191" s="15" t="s">
         <v>57</v>
@@ -8177,15 +8177,15 @@
         <v>178</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
       <c r="F192" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G192" s="15" t="s">
         <v>57</v>
@@ -8196,15 +8196,15 @@
         <v>179</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G193" s="15" t="s">
         <v>57</v>
@@ -8215,15 +8215,15 @@
         <v>180</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
       <c r="F194" s="14" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G194" s="15" t="s">
         <v>57</v>
@@ -8234,34 +8234,34 @@
         <v>181</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
       <c r="F195" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G195" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196">
+      <c r="A196" s="10">
         <v>182</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
       <c r="F196" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G196" s="15" t="s">
         <v>57</v>
@@ -8272,99 +8272,99 @@
         <v>183</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="D197" s="14"/>
+        <v>356</v>
+      </c>
+      <c r="D197" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E197" s="14"/>
       <c r="F197" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G197" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="10">
+      <c r="A198">
         <v>184</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D198" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E198" s="14"/>
       <c r="F198" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G198" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199">
+      <c r="A199" s="10">
         <v>185</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D199" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E199" s="14"/>
       <c r="F199" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G199" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200">
+      <c r="A200" s="10">
         <v>186</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E200" s="14"/>
       <c r="F200" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G200" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="10">
+      <c r="A201">
         <v>187</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C201" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="D201" s="14" t="s">
-        <v>44</v>
-      </c>
+      <c r="D201" s="14"/>
       <c r="E201" s="14"/>
       <c r="F201" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G201" s="15" t="s">
         <v>57</v>
@@ -8375,34 +8375,34 @@
         <v>188</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
       <c r="F202" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G202" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203">
+      <c r="A203" s="10">
         <v>189</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>368</v>
+        <v>398</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>362</v>
+        <v>399</v>
       </c>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
       <c r="F203" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G203" s="15" t="s">
         <v>57</v>
@@ -8413,15 +8413,15 @@
         <v>190</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
       <c r="F204" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G204" s="15" t="s">
         <v>57</v>
@@ -8432,15 +8432,15 @@
         <v>191</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
       <c r="F205" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G205" s="15" t="s">
         <v>57</v>
@@ -8451,15 +8451,15 @@
         <v>192</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
       <c r="F206" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G206" s="15" t="s">
         <v>57</v>
@@ -8470,34 +8470,34 @@
         <v>193</v>
       </c>
       <c r="B207" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="C207" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="C207" s="14" t="s">
-        <v>387</v>
       </c>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
       <c r="F207" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G207" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208">
+      <c r="A208" s="10">
         <v>194</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
       <c r="F208" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G208" s="15" t="s">
         <v>57</v>
@@ -8508,72 +8508,72 @@
         <v>195</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
       <c r="F209" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G209" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="10">
+      <c r="A210">
         <v>196</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
       <c r="F210" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G210" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A211">
+      <c r="A211" s="10">
         <v>197</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
       <c r="F211" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G211" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212">
+      <c r="A212" s="10">
         <v>198</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C212" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
       <c r="F212" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G212" s="15" t="s">
         <v>57</v>
@@ -8584,22 +8584,22 @@
         <v>199</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>402</v>
+        <v>530</v>
       </c>
       <c r="C213" s="14" t="s">
-        <v>403</v>
+        <v>531</v>
       </c>
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
       <c r="F213" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G213" s="15" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A14:I213" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
+  <autoFilter ref="A14:I212" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>

<commit_message>
GeoTools_cfg.xlsx: Feld Tra.BasisUeb eingeführt
</commit_message>
<xml_diff>
--- a/bin/GeoTools_cfg.xlsx
+++ b/bin/GeoTools_cfg.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Office\Office365\xlstart\GeoToolsRes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\LRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B3AA43-8441-46C5-A3DF-EE777A384BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{678BAA68-87DD-4B80-8AFB-80DFD2DA21BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-110" windowWidth="24450" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4210" yWindow="440" windowWidth="20090" windowHeight="12500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="13" r:id="rId1"/>
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$I$212</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$A$14:$I$214</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -373,7 +373,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="534">
   <si>
     <t>GK.X</t>
   </si>
@@ -2055,6 +2055,12 @@
   </si>
   <si>
     <t>LRP GeometrieTrend (k = konstant, v = variabel, ? = unbekannt)</t>
+  </si>
+  <si>
+    <t>Tra.BasisUeb</t>
+  </si>
+  <si>
+    <t>Basis für Überhöhung</t>
   </si>
 </sst>
 </file>
@@ -4181,10 +4187,10 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I213"/>
+  <dimension ref="A1:I214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -6471,13 +6477,13 @@
         <v>100</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>18</v>
+        <v>532</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>29</v>
+        <v>533</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E114" s="14"/>
       <c r="F114" s="14" t="s">
@@ -6486,25 +6492,19 @@
       <c r="G114" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H114" s="46" t="s">
-        <v>479</v>
-      </c>
-      <c r="I114" s="46" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="115" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>101</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E115" s="14"/>
       <c r="F115" s="14" t="s">
@@ -6514,21 +6514,21 @@
         <v>57</v>
       </c>
       <c r="H115" s="46" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I115" s="46" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>102</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>527</v>
+        <v>17</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>528</v>
+        <v>28</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>44</v>
@@ -6540,11 +6540,11 @@
       <c r="G116" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H116" s="50" t="s">
-        <v>529</v>
-      </c>
-      <c r="I116" s="50" t="s">
-        <v>472</v>
+      <c r="H116" s="46" t="s">
+        <v>480</v>
+      </c>
+      <c r="I116" s="46" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -6552,10 +6552,10 @@
         <v>103</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>20</v>
+        <v>527</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>328</v>
+        <v>528</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>44</v>
@@ -6568,21 +6568,21 @@
         <v>57</v>
       </c>
       <c r="H117" s="50" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="I117" s="50" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>104</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>330</v>
+        <v>20</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>44</v>
@@ -6595,21 +6595,21 @@
         <v>57</v>
       </c>
       <c r="H118" s="50" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="I118" s="50" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>105</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>428</v>
+        <v>330</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>429</v>
+        <v>329</v>
       </c>
       <c r="D119" s="14" t="s">
         <v>44</v>
@@ -6621,11 +6621,11 @@
       <c r="G119" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H119" s="46" t="s">
-        <v>467</v>
-      </c>
-      <c r="I119" s="46" t="s">
-        <v>473</v>
+      <c r="H119" s="50" t="s">
+        <v>525</v>
+      </c>
+      <c r="I119" s="50" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6633,10 +6633,10 @@
         <v>106</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D120" s="14" t="s">
         <v>44</v>
@@ -6649,7 +6649,7 @@
         <v>57</v>
       </c>
       <c r="H120" s="46" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I120" s="46" t="s">
         <v>473</v>
@@ -6660,10 +6660,10 @@
         <v>107</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>19</v>
+        <v>430</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="D121" s="14" t="s">
         <v>44</v>
@@ -6676,7 +6676,7 @@
         <v>57</v>
       </c>
       <c r="H121" s="46" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="I121" s="46" t="s">
         <v>473</v>
@@ -6687,10 +6687,10 @@
         <v>108</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>418</v>
+        <v>19</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D122" s="14" t="s">
         <v>44</v>
@@ -6703,7 +6703,7 @@
         <v>57</v>
       </c>
       <c r="H122" s="46" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I122" s="46" t="s">
         <v>473</v>
@@ -6714,10 +6714,10 @@
         <v>109</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>38</v>
+        <v>418</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>27</v>
+        <v>419</v>
       </c>
       <c r="D123" s="14" t="s">
         <v>44</v>
@@ -6730,7 +6730,7 @@
         <v>57</v>
       </c>
       <c r="H123" s="46" t="s">
-        <v>475</v>
+        <v>493</v>
       </c>
       <c r="I123" s="46" t="s">
         <v>473</v>
@@ -6741,13 +6741,13 @@
         <v>110</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>406</v>
+        <v>38</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>407</v>
+        <v>27</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E124" s="14"/>
       <c r="F124" s="14" t="s">
@@ -6757,7 +6757,7 @@
         <v>57</v>
       </c>
       <c r="H124" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I124" s="46" t="s">
         <v>473</v>
@@ -6768,13 +6768,13 @@
         <v>111</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>383</v>
+        <v>407</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E125" s="14"/>
       <c r="F125" s="14" t="s">
@@ -6784,7 +6784,7 @@
         <v>57</v>
       </c>
       <c r="H125" s="46" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I125" s="46" t="s">
         <v>473</v>
@@ -6795,10 +6795,10 @@
         <v>112</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D126" s="14" t="s">
         <v>44</v>
@@ -6811,7 +6811,7 @@
         <v>57</v>
       </c>
       <c r="H126" s="46" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I126" s="46" t="s">
         <v>473</v>
@@ -6822,12 +6822,14 @@
         <v>113</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="D127" s="14"/>
+        <v>382</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E127" s="14"/>
       <c r="F127" s="14" t="s">
         <v>25</v>
@@ -6835,20 +6837,24 @@
       <c r="G127" s="15" t="s">
         <v>57</v>
       </c>
+      <c r="H127" s="46" t="s">
+        <v>478</v>
+      </c>
+      <c r="I127" s="46" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="128" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>114</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="D128" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="D128" s="14"/>
       <c r="E128" s="14"/>
       <c r="F128" s="14" t="s">
         <v>25</v>
@@ -6862,10 +6868,10 @@
         <v>115</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>409</v>
+        <v>368</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>410</v>
+        <v>369</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>44</v>
@@ -6877,22 +6883,16 @@
       <c r="G129" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H129" s="46" t="s">
-        <v>499</v>
-      </c>
-      <c r="I129" s="46" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="130" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>116</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>44</v>
@@ -6905,7 +6905,7 @@
         <v>57</v>
       </c>
       <c r="H130" s="46" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I130" s="46" t="s">
         <v>473</v>
@@ -6916,10 +6916,10 @@
         <v>117</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>44</v>
@@ -6932,7 +6932,7 @@
         <v>57</v>
       </c>
       <c r="H131" s="46" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I131" s="46" t="s">
         <v>473</v>
@@ -6943,10 +6943,10 @@
         <v>118</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D132" s="14" t="s">
         <v>44</v>
@@ -6959,7 +6959,7 @@
         <v>57</v>
       </c>
       <c r="H132" s="46" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I132" s="46" t="s">
         <v>473</v>
@@ -6970,10 +6970,10 @@
         <v>119</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D133" s="14" t="s">
         <v>44</v>
@@ -6986,7 +6986,7 @@
         <v>57</v>
       </c>
       <c r="H133" s="46" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I133" s="46" t="s">
         <v>473</v>
@@ -6997,12 +6997,14 @@
         <v>120</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="D134" s="14"/>
+        <v>416</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E134" s="14"/>
       <c r="F134" s="14" t="s">
         <v>25</v>
@@ -7011,10 +7013,10 @@
         <v>57</v>
       </c>
       <c r="H134" s="46" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I134" s="46" t="s">
-        <v>498</v>
+        <v>473</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7022,10 +7024,10 @@
         <v>121</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
@@ -7036,7 +7038,7 @@
         <v>57</v>
       </c>
       <c r="H135" s="46" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I135" s="46" t="s">
         <v>498</v>
@@ -7047,10 +7049,10 @@
         <v>122</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
@@ -7061,7 +7063,7 @@
         <v>57</v>
       </c>
       <c r="H136" s="46" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I136" s="46" t="s">
         <v>498</v>
@@ -7072,10 +7074,10 @@
         <v>123</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
@@ -7086,7 +7088,7 @@
         <v>57</v>
       </c>
       <c r="H137" s="46" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I137" s="46" t="s">
         <v>498</v>
@@ -7097,10 +7099,10 @@
         <v>124</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
@@ -7111,7 +7113,7 @@
         <v>57</v>
       </c>
       <c r="H138" s="46" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I138" s="46" t="s">
         <v>498</v>
@@ -7122,10 +7124,10 @@
         <v>125</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
@@ -7136,7 +7138,7 @@
         <v>57</v>
       </c>
       <c r="H139" s="46" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I139" s="46" t="s">
         <v>498</v>
@@ -7147,10 +7149,10 @@
         <v>126</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D140" s="14"/>
       <c r="E140" s="14"/>
@@ -7161,7 +7163,7 @@
         <v>57</v>
       </c>
       <c r="H140" s="46" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I140" s="46" t="s">
         <v>498</v>
@@ -7172,10 +7174,10 @@
         <v>127</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D141" s="14"/>
       <c r="E141" s="14"/>
@@ -7186,7 +7188,7 @@
         <v>57</v>
       </c>
       <c r="H141" s="46" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I141" s="46" t="s">
         <v>498</v>
@@ -7197,10 +7199,10 @@
         <v>128</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D142" s="14"/>
       <c r="E142" s="14"/>
@@ -7211,7 +7213,7 @@
         <v>57</v>
       </c>
       <c r="H142" s="46" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I142" s="46" t="s">
         <v>498</v>
@@ -7222,26 +7224,24 @@
         <v>129</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>248</v>
+        <v>441</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="D143" s="14"/>
       <c r="E143" s="14"/>
       <c r="F143" s="14" t="s">
-        <v>252</v>
+        <v>25</v>
       </c>
       <c r="G143" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H143" s="46" t="s">
-        <v>486</v>
+        <v>512</v>
       </c>
       <c r="I143" s="46" t="s">
-        <v>472</v>
+        <v>498</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7249,10 +7249,10 @@
         <v>130</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D144" s="14" t="s">
         <v>44</v>
@@ -7265,23 +7265,25 @@
         <v>57</v>
       </c>
       <c r="H144" s="46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I144" s="46" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>131</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D145" s="14"/>
+        <v>251</v>
+      </c>
+      <c r="D145" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E145" s="14"/>
       <c r="F145" s="14" t="s">
         <v>252</v>
@@ -7289,35 +7291,41 @@
       <c r="G145" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H145" s="46" t="s">
+        <v>487</v>
+      </c>
+      <c r="I145" s="46" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>132</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="D146" s="14"/>
       <c r="E146" s="14"/>
       <c r="F146" s="14" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="G146" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="10">
         <v>133</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D147" s="14"/>
       <c r="E147" s="14"/>
@@ -7328,15 +7336,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="10">
+    <row r="148" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148">
         <v>134</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="D148" s="14"/>
       <c r="E148" s="14"/>
@@ -7347,15 +7355,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>135</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
@@ -7366,15 +7374,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150">
+    <row r="150" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="10">
         <v>136</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D150" s="14"/>
       <c r="E150" s="14"/>
@@ -7385,15 +7393,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="10">
+    <row r="151" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151">
         <v>137</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D151" s="14"/>
       <c r="E151" s="14"/>
@@ -7404,19 +7412,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="10">
+    <row r="152" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152">
         <v>138</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="D152" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D152" s="14"/>
       <c r="E152" s="14"/>
       <c r="F152" s="14" t="s">
         <v>217</v>
@@ -7425,17 +7431,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153">
+    <row r="153" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="10">
         <v>139</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="D153" s="14"/>
+        <v>215</v>
+      </c>
+      <c r="D153" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="E153" s="14"/>
       <c r="F153" s="14" t="s">
         <v>217</v>
@@ -7444,15 +7452,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>140</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="D154" s="14"/>
       <c r="E154" s="14"/>
@@ -7463,15 +7471,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="10">
+    <row r="155" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155">
         <v>141</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
@@ -7482,15 +7490,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="10">
         <v>142</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
@@ -7501,15 +7509,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>143</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D157" s="14"/>
       <c r="E157" s="14"/>
@@ -7520,15 +7528,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>144</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D158" s="14"/>
       <c r="E158" s="14"/>
@@ -7539,15 +7547,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="10">
         <v>145</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
@@ -7558,15 +7566,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="10">
+    <row r="160" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160">
         <v>146</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="D160" s="14"/>
       <c r="E160" s="14"/>
@@ -7582,10 +7590,10 @@
         <v>147</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D161" s="14"/>
       <c r="E161" s="14"/>
@@ -7597,18 +7605,16 @@
       </c>
     </row>
     <row r="162" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162">
+      <c r="A162" s="10">
         <v>148</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="D162" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="D162" s="14"/>
       <c r="E162" s="14"/>
       <c r="F162" s="14" t="s">
         <v>217</v>
@@ -7618,16 +7624,18 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="10">
+      <c r="A163">
         <v>149</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="D163" s="14"/>
+        <v>231</v>
+      </c>
+      <c r="D163" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E163" s="14"/>
       <c r="F163" s="14" t="s">
         <v>217</v>
@@ -7637,14 +7645,14 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="10">
+      <c r="A164">
         <v>150</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
@@ -7656,14 +7664,14 @@
       </c>
     </row>
     <row r="165" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165">
+      <c r="A165" s="10">
         <v>151</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
@@ -7679,10 +7687,10 @@
         <v>152</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="D166" s="14"/>
       <c r="E166" s="14"/>
@@ -7694,14 +7702,14 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="10">
+      <c r="A167">
         <v>153</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D167" s="14"/>
       <c r="E167" s="14"/>
@@ -7717,10 +7725,10 @@
         <v>154</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
@@ -7736,15 +7744,15 @@
         <v>155</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>188</v>
+        <v>229</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
       <c r="F169" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G169" s="15" t="s">
         <v>57</v>
@@ -7755,14 +7763,12 @@
         <v>156</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D170" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D170" s="14"/>
       <c r="E170" s="14"/>
       <c r="F170" s="14" t="s">
         <v>216</v>
@@ -7776,12 +7782,14 @@
         <v>157</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D171" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="D171" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E171" s="14"/>
       <c r="F171" s="14" t="s">
         <v>216</v>
@@ -7791,14 +7799,14 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="10">
+      <c r="A172">
         <v>158</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
@@ -7814,14 +7822,12 @@
         <v>159</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>299</v>
+        <v>186</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="D173" s="14"/>
       <c r="E173" s="14"/>
       <c r="F173" s="14" t="s">
         <v>216</v>
@@ -7831,33 +7837,35 @@
       </c>
     </row>
     <row r="174" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174">
+      <c r="A174" s="10">
         <v>160</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="D174" s="14"/>
+        <v>300</v>
+      </c>
+      <c r="D174" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E174" s="14"/>
       <c r="F174" s="14" t="s">
-        <v>311</v>
+        <v>216</v>
       </c>
       <c r="G174" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="10">
+      <c r="A175">
         <v>161</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
@@ -7869,14 +7877,14 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="10">
+      <c r="A176">
         <v>162</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
@@ -7888,14 +7896,14 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177">
+      <c r="A177" s="10">
         <v>163</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
@@ -7911,10 +7919,10 @@
         <v>164</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
@@ -7926,14 +7934,14 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="10">
+      <c r="A179">
         <v>165</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
@@ -7949,10 +7957,10 @@
         <v>166</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D180" s="14"/>
       <c r="E180" s="14"/>
@@ -7968,10 +7976,10 @@
         <v>167</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D181" s="14"/>
       <c r="E181" s="14"/>
@@ -7987,15 +7995,15 @@
         <v>168</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
       <c r="F182" s="14" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
       <c r="G182" s="15" t="s">
         <v>57</v>
@@ -8006,10 +8014,10 @@
         <v>169</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>375</v>
+        <v>340</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>376</v>
+        <v>337</v>
       </c>
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
@@ -8021,14 +8029,14 @@
       </c>
     </row>
     <row r="184" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="10">
+      <c r="A184">
         <v>170</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
@@ -8044,10 +8052,10 @@
         <v>171</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>338</v>
+        <v>378</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>335</v>
+        <v>377</v>
       </c>
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
@@ -8059,14 +8067,14 @@
       </c>
     </row>
     <row r="186" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186">
+      <c r="A186" s="10">
         <v>172</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>521</v>
+        <v>338</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>516</v>
+        <v>335</v>
       </c>
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
@@ -8078,14 +8086,14 @@
       </c>
     </row>
     <row r="187" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" s="10">
+      <c r="A187">
         <v>173</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C187" s="14" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D187" s="14"/>
       <c r="E187" s="14"/>
@@ -8097,14 +8105,14 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="10">
+      <c r="A188">
         <v>174</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C188" s="14" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D188" s="14"/>
       <c r="E188" s="14"/>
@@ -8116,14 +8124,14 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189">
+      <c r="A189" s="10">
         <v>175</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>339</v>
+        <v>519</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>336</v>
+        <v>520</v>
       </c>
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
@@ -8139,10 +8147,10 @@
         <v>176</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C190" s="14" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
@@ -8154,14 +8162,14 @@
       </c>
     </row>
     <row r="191" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="10">
+      <c r="A191">
         <v>177</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
@@ -8177,10 +8185,10 @@
         <v>178</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
@@ -8196,10 +8204,10 @@
         <v>179</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
@@ -8215,15 +8223,15 @@
         <v>180</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
       <c r="F194" s="14" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G194" s="15" t="s">
         <v>57</v>
@@ -8234,10 +8242,10 @@
         <v>181</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D195" s="14"/>
       <c r="E195" s="14"/>
@@ -8249,14 +8257,14 @@
       </c>
     </row>
     <row r="196" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="10">
+      <c r="A196">
         <v>182</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
@@ -8272,14 +8280,12 @@
         <v>183</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="D197" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>355</v>
+      </c>
+      <c r="D197" s="14"/>
       <c r="E197" s="14"/>
       <c r="F197" s="14" t="s">
         <v>333</v>
@@ -8289,14 +8295,14 @@
       </c>
     </row>
     <row r="198" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198">
+      <c r="A198" s="10">
         <v>184</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D198" s="14" t="s">
         <v>44</v>
@@ -8310,14 +8316,14 @@
       </c>
     </row>
     <row r="199" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="10">
+      <c r="A199">
         <v>185</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D199" s="14" t="s">
         <v>44</v>
@@ -8331,14 +8337,14 @@
       </c>
     </row>
     <row r="200" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="10">
+      <c r="A200">
         <v>186</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D200" s="14" t="s">
         <v>44</v>
@@ -8352,16 +8358,18 @@
       </c>
     </row>
     <row r="201" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201">
+      <c r="A201" s="10">
         <v>187</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="D201" s="14"/>
+        <v>359</v>
+      </c>
+      <c r="D201" s="14" t="s">
+        <v>44</v>
+      </c>
       <c r="E201" s="14"/>
       <c r="F201" s="14" t="s">
         <v>333</v>
@@ -8375,10 +8383,10 @@
         <v>188</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
@@ -8390,14 +8398,14 @@
       </c>
     </row>
     <row r="203" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="10">
+      <c r="A203">
         <v>189</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>398</v>
+        <v>366</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
@@ -8413,10 +8421,10 @@
         <v>190</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>371</v>
+        <v>398</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>373</v>
+        <v>399</v>
       </c>
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
@@ -8432,10 +8440,10 @@
         <v>191</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
@@ -8451,10 +8459,10 @@
         <v>192</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
@@ -8470,10 +8478,10 @@
         <v>193</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D207" s="14"/>
       <c r="E207" s="14"/>
@@ -8485,14 +8493,14 @@
       </c>
     </row>
     <row r="208" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="10">
+      <c r="A208">
         <v>194</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D208" s="14"/>
       <c r="E208" s="14"/>
@@ -8508,10 +8516,10 @@
         <v>195</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
@@ -8523,14 +8531,14 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210">
+      <c r="A210" s="10">
         <v>196</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
@@ -8542,14 +8550,14 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A211" s="10">
+      <c r="A211">
         <v>197</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
@@ -8561,14 +8569,14 @@
       </c>
     </row>
     <row r="212" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="10">
+      <c r="A212">
         <v>198</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C212" s="14" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
@@ -8584,10 +8592,10 @@
         <v>199</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>530</v>
+        <v>400</v>
       </c>
       <c r="C213" s="14" t="s">
-        <v>531</v>
+        <v>401</v>
       </c>
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
@@ -8598,8 +8606,27 @@
         <v>57</v>
       </c>
     </row>
+    <row r="214" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>200</v>
+      </c>
+      <c r="B214" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="C214" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="D214" s="14"/>
+      <c r="E214" s="14"/>
+      <c r="F214" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G214" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A14:I212" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
+  <autoFilter ref="A14:I214" xr:uid="{358D2219-C7E6-472B-B9A0-CD62126A65EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B63:F67">
     <sortCondition ref="B63:B67"/>
   </sortState>

</xml_diff>